<commit_message>
New Launch Validation Codes
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release Team Verification Suite\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B93D86-0B25-434E-B433-ADB56324C20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A4837B-B869-4C11-A725-5721DA196F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="153">
   <si>
     <t>Customer Name</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>River City Medical Group ACO</t>
+  </si>
+  <si>
+    <t>Customer Not in List</t>
   </si>
 </sst>
 </file>
@@ -571,10 +574,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -919,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -932,165 +934,165 @@
     <col min="4" max="4" width="34.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2">
+        <v>99999</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>99999</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="1">
         <v>2400</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="1">
         <v>2400</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="1">
         <v>1500</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="1">
         <v>1500</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="1">
         <v>1500</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="1">
         <v>1500</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="1">
         <v>3700</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="1">
         <v>3700</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="1">
         <v>3700</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="1">
         <v>2200</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>99999</v>
-      </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2">
-        <v>4200</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1098,494 +1100,494 @@
       <c r="D12">
         <v>99999</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4200</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>99999</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="1">
         <v>1600</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="1">
         <v>1600</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B16" s="1">
         <v>1600</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="1">
         <v>1600</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="1">
         <v>1600</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="1">
         <v>4700</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>12</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>99999</v>
       </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B20" s="1">
         <v>3200</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B21" s="1">
         <v>3200</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="1">
         <v>3200</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B23" s="1">
         <v>3100</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="1">
         <v>3100</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="1">
         <v>3100</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B26" s="1">
         <v>1700</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="1">
         <v>1700</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B28" s="1">
         <v>1700</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="1">
         <v>2900</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B30" s="1">
         <v>2900</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="1">
         <v>2900</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="1">
         <v>1800</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="1">
         <v>1800</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="1">
         <v>1800</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B35" s="1">
         <v>1800</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D35" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B36" s="1">
         <v>4300</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B37" s="1">
         <v>4300</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B38" s="1">
         <v>3000</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D38" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B39" s="1">
         <v>3000</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B40" s="1">
         <v>3000</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B41" s="1">
         <v>3000</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D41" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B42" s="1">
         <v>3500</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>5</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D42" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B43" s="1">
         <v>3500</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B44" s="1">
         <v>3500</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B45" s="1">
         <v>200</v>
-      </c>
-      <c r="C44" t="s">
-        <v>12</v>
-      </c>
-      <c r="D44">
-        <v>99999</v>
-      </c>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="2">
-        <v>3600</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
@@ -1593,164 +1595,164 @@
       <c r="D45">
         <v>99999</v>
       </c>
-      <c r="E45" s="2"/>
+      <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="1">
+        <v>3600</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>99999</v>
+      </c>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B47" s="1">
         <v>4600</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D47" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B48" s="1">
         <v>4600</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D48" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B49" s="1">
         <v>4600</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D49" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B50" s="1">
         <v>150</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>5</v>
       </c>
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B51" s="1">
         <v>150</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B52" s="1">
         <v>150</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B53" s="1">
         <v>150</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>15</v>
       </c>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B54" s="1">
         <v>150</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B55" s="1">
         <v>2700</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D55" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B56" s="1">
         <v>2700</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D56" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B57" s="1">
         <v>2000</v>
-      </c>
-      <c r="C56" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56">
-        <v>99999</v>
-      </c>
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" s="2">
-        <v>2100</v>
       </c>
       <c r="C57" t="s">
         <v>12</v>
@@ -1758,119 +1760,119 @@
       <c r="D57">
         <v>99999</v>
       </c>
-      <c r="E57" s="2"/>
+      <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2100</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58">
+        <v>99999</v>
+      </c>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B59" s="1">
         <v>5600</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D59" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B60">
         <v>2600</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>12</v>
       </c>
-      <c r="D59">
+      <c r="D60">
         <v>99999</v>
       </c>
-      <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B61" s="1">
         <v>1100</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D61" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B62" s="1">
         <v>1100</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D62" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B63" s="1">
         <v>1100</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D63" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B64" s="1">
         <v>1100</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D64" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B65" s="1">
         <v>3300</v>
-      </c>
-      <c r="C64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64">
-        <v>99999</v>
-      </c>
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B65" s="2">
-        <v>5100</v>
       </c>
       <c r="C65" t="s">
         <v>12</v>
@@ -1878,14 +1880,14 @@
       <c r="D65">
         <v>99999</v>
       </c>
-      <c r="E65" s="2"/>
+      <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B66" s="2">
-        <v>2800</v>
+      <c r="A66" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" s="1">
+        <v>5100</v>
       </c>
       <c r="C66" t="s">
         <v>12</v>
@@ -1893,14 +1895,14 @@
       <c r="D66">
         <v>99999</v>
       </c>
-      <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B67" s="2">
-        <v>5200</v>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" s="1">
+        <v>2800</v>
       </c>
       <c r="C67" t="s">
         <v>12</v>
@@ -1908,14 +1910,14 @@
       <c r="D67">
         <v>99999</v>
       </c>
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B68" s="2">
-        <v>4800</v>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B68" s="1">
+        <v>5200</v>
       </c>
       <c r="C68" t="s">
         <v>12</v>
@@ -1923,14 +1925,14 @@
       <c r="D68">
         <v>99999</v>
       </c>
-      <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B69" s="2">
-        <v>5300</v>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" s="1">
+        <v>4800</v>
       </c>
       <c r="C69" t="s">
         <v>12</v>
@@ -1938,14 +1940,14 @@
       <c r="D69">
         <v>99999</v>
       </c>
-      <c r="E69" s="2"/>
+      <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B70" s="2">
-        <v>4900</v>
+      <c r="A70" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B70" s="1">
+        <v>5300</v>
       </c>
       <c r="C70" t="s">
         <v>12</v>
@@ -1953,14 +1955,14 @@
       <c r="D70">
         <v>99999</v>
       </c>
-      <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B71" s="2">
-        <v>4100</v>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="1">
+        <v>4900</v>
       </c>
       <c r="C71" t="s">
         <v>12</v>
@@ -1968,14 +1970,14 @@
       <c r="D71">
         <v>99999</v>
       </c>
-      <c r="E71" s="2"/>
+      <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B72" s="2">
-        <v>5000</v>
+      <c r="A72" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" s="1">
+        <v>4100</v>
       </c>
       <c r="C72" t="s">
         <v>12</v>
@@ -1983,14 +1985,14 @@
       <c r="D72">
         <v>99999</v>
       </c>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B73" s="2">
-        <v>4500</v>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" s="1">
+        <v>5000</v>
       </c>
       <c r="C73" t="s">
         <v>12</v>
@@ -1998,924 +2000,939 @@
       <c r="D73">
         <v>99999</v>
       </c>
-      <c r="E73" s="2"/>
+      <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" s="1">
+        <v>4500</v>
+      </c>
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74">
+        <v>99999</v>
+      </c>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B75" s="1">
         <v>3400</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="D75" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E74" s="2"/>
-    </row>
-    <row r="75" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B76" s="1">
         <v>3400</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="D76" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E75" s="2"/>
-    </row>
-    <row r="76" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B77" s="1">
         <v>3400</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>9</v>
       </c>
-      <c r="D76" s="6" t="s">
+      <c r="D77" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E76" s="2"/>
-    </row>
-    <row r="77" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B78" s="1">
         <v>3400</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>15</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="D78" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E77" s="2"/>
-    </row>
-    <row r="78" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B79" s="1">
         <v>3400</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C79" t="s">
         <v>6</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="D79" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E78" s="2"/>
-    </row>
-    <row r="79" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B80" s="1">
         <v>1200</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>48</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D80" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E79" s="2"/>
-    </row>
-    <row r="80" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B81" s="1">
         <v>1200</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D81" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E80" s="2"/>
-    </row>
-    <row r="81" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B82" s="1">
         <v>1200</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>8</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="D82" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E81" s="2"/>
-    </row>
-    <row r="82" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B83" s="1">
         <v>1200</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>9</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D83" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E82" s="2"/>
-    </row>
-    <row r="83" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B84" s="1">
         <v>1400</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>48</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D84" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E83" s="2"/>
-    </row>
-    <row r="84" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B85" s="1">
         <v>1400</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>5</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="D85" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E84" s="2"/>
-    </row>
-    <row r="85" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="3" t="s">
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B86" s="1">
         <v>1400</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="D86" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E85" s="2"/>
-    </row>
-    <row r="86" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B87" s="1">
         <v>1400</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>15</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D87" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E86" s="2"/>
-    </row>
-    <row r="87" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B88" s="1">
         <v>3900</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>5</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="D88" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E87" s="2"/>
-    </row>
-    <row r="88" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B89" s="1">
         <v>3900</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>9</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D89" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E88" s="2"/>
-    </row>
-    <row r="89" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B90" s="1">
         <v>3900</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>15</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D90" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E89" s="2"/>
-    </row>
-    <row r="90" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B91" s="1">
         <v>3900</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="6" t="s">
+      <c r="D91" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E90" s="2"/>
-    </row>
-    <row r="91" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B92" s="1">
         <v>3800</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>5</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D92" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E91" s="2"/>
-    </row>
-    <row r="92" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B93" s="1">
         <v>3800</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>15</v>
       </c>
-      <c r="D92" s="8" t="s">
+      <c r="D93" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E92" s="2"/>
-    </row>
-    <row r="93" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B94" s="1">
         <v>1300</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>5</v>
       </c>
-      <c r="D93" s="6" t="s">
+      <c r="D94" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E93" s="2"/>
-    </row>
-    <row r="94" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3" t="s">
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B95" s="1">
         <v>1300</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>8</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="D95" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E94" s="2"/>
-    </row>
-    <row r="95" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B96" s="1">
         <v>1300</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>9</v>
       </c>
-      <c r="D95" s="6" t="s">
+      <c r="D96" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E95" s="2"/>
-    </row>
-    <row r="96" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B97" s="1">
         <v>1300</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>15</v>
       </c>
-      <c r="D96" s="6" t="s">
+      <c r="D97" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E96" s="2"/>
-    </row>
-    <row r="97" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B98" s="1">
         <v>1300</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>6</v>
       </c>
-      <c r="D97" s="6" t="s">
+      <c r="D98" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E97" s="2"/>
-    </row>
-    <row r="98" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B99" s="1">
         <v>2500</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>48</v>
       </c>
-      <c r="D98" s="11" t="s">
+      <c r="D99" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E98" s="2"/>
-    </row>
-    <row r="99" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="3" t="s">
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B100" s="1">
         <v>2500</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>5</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D100" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="E99" s="2"/>
-    </row>
-    <row r="100" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="s">
+      <c r="E100" s="1"/>
+    </row>
+    <row r="101" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B101" s="1">
         <v>2500</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>8</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="D101" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E100" s="2"/>
-    </row>
-    <row r="101" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B102" s="1">
         <v>6000</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>5</v>
       </c>
-      <c r="D101" s="6" t="s">
+      <c r="D102" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="E101" s="2"/>
-    </row>
-    <row r="102" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B103" s="1">
         <v>6000</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>8</v>
       </c>
-      <c r="D102" s="6" t="s">
+      <c r="D103" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E102" s="2"/>
-    </row>
-    <row r="103" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="3" t="s">
+      <c r="E103" s="1"/>
+    </row>
+    <row r="104" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B104" s="1">
         <v>6000</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>15</v>
       </c>
-      <c r="D103" s="6" t="s">
+      <c r="D104" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E103" s="2"/>
-    </row>
-    <row r="104" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="3" t="s">
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B105" s="1">
         <v>5400</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>12</v>
       </c>
-      <c r="D104" s="6">
+      <c r="D105" s="5">
         <v>99999</v>
       </c>
-      <c r="E104" s="2"/>
-    </row>
-    <row r="105" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
+      <c r="E105" s="1"/>
+    </row>
+    <row r="106" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B105" s="2">
+      <c r="B106" s="1">
         <v>1000</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>5</v>
       </c>
-      <c r="D105" s="6" t="s">
+      <c r="D106" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E105" s="2"/>
-    </row>
-    <row r="106" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
+      <c r="E106" s="1"/>
+    </row>
+    <row r="107" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B107" s="1">
         <v>1000</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>15</v>
       </c>
-      <c r="D106" s="6" t="s">
+      <c r="D107" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E106" s="2"/>
-    </row>
-    <row r="107" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="3" t="s">
+      <c r="E107" s="1"/>
+    </row>
+    <row r="108" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B108" s="1">
         <v>1000</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>6</v>
       </c>
-      <c r="D107" s="6" t="s">
+      <c r="D108" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E107" s="2"/>
-    </row>
-    <row r="108" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
+      <c r="E108" s="1"/>
+    </row>
+    <row r="109" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B109" s="1">
         <v>1900</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C109" t="s">
         <v>5</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="D109" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E108" s="2"/>
-    </row>
-    <row r="109" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
+      <c r="E109" s="1"/>
+    </row>
+    <row r="110" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B110" s="1">
         <v>1900</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>8</v>
       </c>
-      <c r="D109" s="6" t="s">
+      <c r="D110" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E109" s="2"/>
-    </row>
-    <row r="110" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B111" s="1">
         <v>1900</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>9</v>
       </c>
-      <c r="D110" s="6" t="s">
+      <c r="D111" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E110" s="2"/>
-    </row>
-    <row r="111" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
+      <c r="E111" s="1"/>
+    </row>
+    <row r="112" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B112" s="1">
         <v>1900</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>15</v>
       </c>
-      <c r="D111" s="6" t="s">
+      <c r="D112" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E111" s="2"/>
-    </row>
-    <row r="112" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="3" t="s">
+      <c r="E112" s="1"/>
+    </row>
+    <row r="113" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B113" s="1">
         <v>1900</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C113" t="s">
         <v>6</v>
       </c>
-      <c r="D112" s="6" t="s">
+      <c r="D113" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E112" s="2"/>
-    </row>
-    <row r="113" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="3" t="s">
+      <c r="E113" s="1"/>
+    </row>
+    <row r="114" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B114" s="1">
         <v>4000</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>5</v>
       </c>
-      <c r="D113" s="6" t="s">
+      <c r="D114" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E113" s="2"/>
-    </row>
-    <row r="114" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
+      <c r="E114" s="1"/>
+    </row>
+    <row r="115" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B115" s="1">
         <v>4000</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C115" t="s">
         <v>9</v>
       </c>
-      <c r="D114" s="6" t="s">
+      <c r="D115" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E114" s="2"/>
-    </row>
-    <row r="115" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B116" s="1">
         <v>4000</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C116" t="s">
         <v>15</v>
       </c>
-      <c r="D115" s="6" t="s">
+      <c r="D116" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E115" s="2"/>
-    </row>
-    <row r="116" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="3" t="s">
+      <c r="E116" s="1"/>
+    </row>
+    <row r="117" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B117" s="1">
         <v>6500</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>48</v>
       </c>
-      <c r="D116" s="12" t="s">
+      <c r="D117" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E116" s="2"/>
-    </row>
-    <row r="117" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="3" t="s">
+      <c r="E117" s="1"/>
+    </row>
+    <row r="118" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B118" s="1">
         <v>6500</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C118" t="s">
         <v>5</v>
       </c>
-      <c r="D117" s="12" t="s">
+      <c r="D118" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="E117" s="2"/>
-    </row>
-    <row r="118" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="3" t="s">
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B118" s="2">
+      <c r="B119" s="1">
         <v>6500</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" t="s">
         <v>8</v>
       </c>
-      <c r="D118" s="12" t="s">
+      <c r="D119" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E118" s="2"/>
-    </row>
-    <row r="119" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="3" t="s">
+      <c r="E119" s="1"/>
+    </row>
+    <row r="120" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B120" s="1">
         <v>6500</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" t="s">
         <v>9</v>
       </c>
-      <c r="D119" s="6" t="s">
+      <c r="D120" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E119" s="2"/>
-    </row>
-    <row r="120" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="3" t="s">
+      <c r="E120" s="1"/>
+    </row>
+    <row r="121" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B121" s="1">
         <v>6500</v>
       </c>
-      <c r="C120" s="10" t="s">
+      <c r="C121" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D120" s="12" t="s">
+      <c r="D121" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="E120" s="2"/>
-    </row>
-    <row r="121" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="3" t="s">
+      <c r="E121" s="1"/>
+    </row>
+    <row r="122" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B122" s="1">
         <v>6500</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C122" t="s">
         <v>6</v>
       </c>
-      <c r="D121" s="12" t="s">
+      <c r="D122" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="E121" s="2"/>
-    </row>
-    <row r="122" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="3" t="s">
+      <c r="E122" s="1"/>
+    </row>
+    <row r="123" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B123" s="1">
         <v>4400</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C123" t="s">
         <v>5</v>
       </c>
-      <c r="D122" s="12"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
+      <c r="D123" s="11"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B124" s="1">
         <v>4400</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C124" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B125" s="1">
         <v>4400</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C125" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="s">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B126" s="1">
         <v>4400</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C126" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B127" s="1">
         <v>4400</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C127" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="A17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="A18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="A19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="A20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="A21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="A32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="A35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="A39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="A42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="A43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="A44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="A45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="A46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="A47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="A48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="A49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="A50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="A51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="A52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="A53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="A54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="A55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="A56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="A57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="A59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="A60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="A61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="A62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="A63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="A64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="A65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="A66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="A67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="A68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="A99" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="A100" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="A101" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="A102" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="A103" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="A105" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="A106" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="A107" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="A108" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="A109" r:id="rId76" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="A110" r:id="rId77" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="A111" r:id="rId78" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="A112" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="A113" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="A114" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="A115" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="A116" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="A117" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="A118" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="A120" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="A121" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="A122" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="A123" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="A124" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="A125" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="A126" r:id="rId92" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="D2" r:id="rId93" display="http://sabose.cu/" xr:uid="{47EDC6A2-E374-4384-83BF-1151296A8B80}"/>
-    <hyperlink ref="D21" r:id="rId94" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{8191FBBF-8854-4C0A-8B84-E84F0CC1A943}"/>
-    <hyperlink ref="D24" r:id="rId95" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{BBD40848-FBCD-4DBE-ADBF-830C639AC43C}"/>
-    <hyperlink ref="D23" r:id="rId96" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{E347D519-C1BE-4E2F-9DE2-4F876CAA1896}"/>
-    <hyperlink ref="D22" r:id="rId97" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{099130F4-96CB-41A1-AF6B-E959DE9F4517}"/>
-    <hyperlink ref="D37" r:id="rId98" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTMwMDAmb3JnSWQ9MTQ2NzU0&amp;person_id=22297698&amp;forPersonCustId=3000" xr:uid="{850A56CE-02C6-4335-82D5-BC8FCA19D520}"/>
-    <hyperlink ref="D40" r:id="rId99" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=21687687&amp;forPersonCustId=3000" xr:uid="{2E221ED3-44BB-4C33-B120-4A5DC7FC4D0C}"/>
-    <hyperlink ref="D41" r:id="rId100" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{90032F47-9BAC-4D8F-9DEB-338BF29E04F2}"/>
-    <hyperlink ref="D42" r:id="rId101" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{1D2F84AA-1DE0-4251-9DAE-1EF798CFEFBC}"/>
-    <hyperlink ref="D43" r:id="rId102" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{AD4A5868-800F-42DC-8BEC-9F2A06319281}"/>
-    <hyperlink ref="D83" r:id="rId103" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=6929346&amp;forPersonCustId=47" xr:uid="{1EBA4DAD-A644-4D69-939A-195D56E5D254}"/>
-    <hyperlink ref="D84" r:id="rId104" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36889637&amp;forPersonCustId=1400" xr:uid="{AE6AD973-8B2E-45FA-B623-EA01EBEE0AFD}"/>
-    <hyperlink ref="D85" r:id="rId105" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=22433553&amp;forPersonCustId=1400" xr:uid="{962BF6F0-F8E6-4D8B-B56F-CDB12A596BA0}"/>
-    <hyperlink ref="D91" r:id="rId106" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{7FD4B6CF-752F-4666-818B-8BA80FC216F5}"/>
-    <hyperlink ref="D92" r:id="rId107" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{30966F6F-B77C-4914-AB8D-A15DBD0329F5}"/>
-    <hyperlink ref="D108" r:id="rId108" display="http://puchakraborty.cm/" xr:uid="{FB84B2F6-939B-44E5-95B2-C963662FBD0C}"/>
-    <hyperlink ref="A119" r:id="rId109" xr:uid="{2D237A29-BE80-4D01-9992-C2BEB4FB6FC3}"/>
-    <hyperlink ref="A98" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="A97" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="A96" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="A95" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="A94" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="A93" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="A92" r:id="rId116" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="A91" r:id="rId117" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="A90" r:id="rId118" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="A89" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="A88" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="A87" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="A86" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="A85" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="A84" r:id="rId124" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="A83" r:id="rId125" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="A82" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="A81" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="A80" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="A79" r:id="rId129" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="A78" r:id="rId130" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="A77" r:id="rId131" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="A76" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="A75" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="A74" r:id="rId134" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="A73" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="A72" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="A71" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="A70" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="A43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="A45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="A54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="A55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="A56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="A57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="A58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="A60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="A61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="A62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="A63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="A64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="A65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="A66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="A67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="A68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="A69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="A100" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="A101" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="A102" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="A103" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="A104" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="A106" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="A107" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="A108" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="A109" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="A110" r:id="rId76" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="A111" r:id="rId77" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="A112" r:id="rId78" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="A113" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="A114" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="A115" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="A116" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="A117" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="A118" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="A119" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="A121" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="A122" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="A123" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="A124" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="A125" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="A126" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="A127" r:id="rId92" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="D3" r:id="rId93" display="http://sabose.cu/" xr:uid="{47EDC6A2-E374-4384-83BF-1151296A8B80}"/>
+    <hyperlink ref="D22" r:id="rId94" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{8191FBBF-8854-4C0A-8B84-E84F0CC1A943}"/>
+    <hyperlink ref="D25" r:id="rId95" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{BBD40848-FBCD-4DBE-ADBF-830C639AC43C}"/>
+    <hyperlink ref="D24" r:id="rId96" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{E347D519-C1BE-4E2F-9DE2-4F876CAA1896}"/>
+    <hyperlink ref="D23" r:id="rId97" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{099130F4-96CB-41A1-AF6B-E959DE9F4517}"/>
+    <hyperlink ref="D38" r:id="rId98" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTMwMDAmb3JnSWQ9MTQ2NzU0&amp;person_id=22297698&amp;forPersonCustId=3000" xr:uid="{850A56CE-02C6-4335-82D5-BC8FCA19D520}"/>
+    <hyperlink ref="D41" r:id="rId99" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=21687687&amp;forPersonCustId=3000" xr:uid="{2E221ED3-44BB-4C33-B120-4A5DC7FC4D0C}"/>
+    <hyperlink ref="D42" r:id="rId100" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{90032F47-9BAC-4D8F-9DEB-338BF29E04F2}"/>
+    <hyperlink ref="D43" r:id="rId101" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{1D2F84AA-1DE0-4251-9DAE-1EF798CFEFBC}"/>
+    <hyperlink ref="D44" r:id="rId102" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{AD4A5868-800F-42DC-8BEC-9F2A06319281}"/>
+    <hyperlink ref="D84" r:id="rId103" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=6929346&amp;forPersonCustId=47" xr:uid="{1EBA4DAD-A644-4D69-939A-195D56E5D254}"/>
+    <hyperlink ref="D85" r:id="rId104" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36889637&amp;forPersonCustId=1400" xr:uid="{AE6AD973-8B2E-45FA-B623-EA01EBEE0AFD}"/>
+    <hyperlink ref="D86" r:id="rId105" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=22433553&amp;forPersonCustId=1400" xr:uid="{962BF6F0-F8E6-4D8B-B56F-CDB12A596BA0}"/>
+    <hyperlink ref="D92" r:id="rId106" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{7FD4B6CF-752F-4666-818B-8BA80FC216F5}"/>
+    <hyperlink ref="D93" r:id="rId107" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{30966F6F-B77C-4914-AB8D-A15DBD0329F5}"/>
+    <hyperlink ref="D109" r:id="rId108" display="http://puchakraborty.cm/" xr:uid="{FB84B2F6-939B-44E5-95B2-C963662FBD0C}"/>
+    <hyperlink ref="A120" r:id="rId109" xr:uid="{2D237A29-BE80-4D01-9992-C2BEB4FB6FC3}"/>
+    <hyperlink ref="A99" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="A98" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="A97" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="A96" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="A95" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="A94" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="A93" r:id="rId116" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="A92" r:id="rId117" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="A91" r:id="rId118" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="A90" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="A89" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="A88" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="A87" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="A86" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="A85" r:id="rId124" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A84" r:id="rId125" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="A83" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="A82" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="A81" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="A80" r:id="rId129" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="A79" r:id="rId130" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="A78" r:id="rId131" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="A77" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A76" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="A75" r:id="rId134" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="A74" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="A73" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="A72" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A71" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId139"/>

</xml_diff>

<commit_message>
Adding SHC and USRC
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA43D91-CD37-4238-B1F0-BEEF31B976D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC17FA3F-FAC7-4F3F-A0E4-7FE6007C0ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="155">
   <si>
     <t>Customer Name</t>
   </si>
@@ -330,6 +330,21 @@
     <t>Omn_horchhay</t>
   </si>
   <si>
+    <t>PDT_rtorres</t>
+  </si>
+  <si>
+    <t>PDT_cclegg</t>
+  </si>
+  <si>
+    <t>pdt_vrodriguez</t>
+  </si>
+  <si>
+    <t>PDT_msebastian</t>
+  </si>
+  <si>
+    <t>PDT_rperez</t>
+  </si>
+  <si>
     <t>dmorales</t>
   </si>
   <si>
@@ -466,6 +481,15 @@
   </si>
   <si>
     <t>River City Medical Group ACO</t>
+  </si>
+  <si>
+    <t>Customer Not in List</t>
+  </si>
+  <si>
+    <t>Stanford Health Care</t>
+  </si>
+  <si>
+    <t>U.S. Renal Care</t>
   </si>
 </sst>
 </file>
@@ -903,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -916,7 +940,7 @@
     <col min="4" max="4" width="34.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -932,44 +956,47 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2400</v>
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2">
+        <v>99999</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>60</v>
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>99999</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>2400</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2400</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1500</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -981,7 +1008,7 @@
         <v>1500</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -993,11 +1020,11 @@
         <v>1500</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1005,22 +1032,19 @@
         <v>1500</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>3700</v>
+        <v>1500</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -1032,10 +1056,10 @@
         <v>3700</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -1047,34 +1071,34 @@
         <v>3700</v>
       </c>
       <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3700</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>2200</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>99999</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <v>4200</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1086,16 +1110,16 @@
     </row>
     <row r="13" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>1600</v>
+        <v>4200</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>65</v>
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>99999</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -1107,10 +1131,10 @@
         <v>1600</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -1122,10 +1146,10 @@
         <v>1600</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -1137,10 +1161,10 @@
         <v>1600</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -1152,40 +1176,40 @@
         <v>1600</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1">
-        <v>4700</v>
+        <v>1600</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>99999</v>
+        <v>6</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
-        <v>3200</v>
+        <v>4700</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>70</v>
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>99999</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -1197,10 +1221,10 @@
         <v>3200</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -1212,25 +1236,25 @@
         <v>3200</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>72</v>
+        <v>8</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
-        <v>3100</v>
+        <v>3200</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -1242,10 +1266,10 @@
         <v>3100</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -1257,25 +1281,25 @@
         <v>3100</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="1">
-        <v>1700</v>
+        <v>3100</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>76</v>
+        <v>15</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="E25" s="1"/>
     </row>
@@ -1287,10 +1311,10 @@
         <v>1700</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26" s="1"/>
     </row>
@@ -1302,25 +1326,25 @@
         <v>1700</v>
       </c>
       <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1700</v>
+      </c>
+      <c r="C28" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="1">
-        <v>2900</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E28" s="1"/>
     </row>
@@ -1332,14 +1356,14 @@
         <v>2900</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -1347,25 +1371,25 @@
         <v>2900</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B31" s="1">
-        <v>1800</v>
+        <v>2900</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>79</v>
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E31" s="1"/>
     </row>
@@ -1377,10 +1401,10 @@
         <v>1800</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" s="1"/>
     </row>
@@ -1392,10 +1416,10 @@
         <v>1800</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -1407,25 +1431,25 @@
         <v>1800</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" s="1">
-        <v>4300</v>
+        <v>1800</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>83</v>
+        <v>6</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="E35" s="1"/>
     </row>
@@ -1437,25 +1461,25 @@
         <v>4300</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" s="1">
-        <v>3000</v>
+        <v>4300</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>85</v>
+        <v>8</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="E37" s="1"/>
     </row>
@@ -1467,10 +1491,10 @@
         <v>3000</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="E38" s="1"/>
     </row>
@@ -1482,10 +1506,10 @@
         <v>3000</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>87</v>
+        <v>8</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="E39" s="1"/>
     </row>
@@ -1497,25 +1521,25 @@
         <v>3000</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>88</v>
+        <v>9</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B41" s="1">
-        <v>3500</v>
+        <v>3000</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E41" s="1"/>
     </row>
@@ -1527,10 +1551,10 @@
         <v>3500</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42" s="1"/>
     </row>
@@ -1542,34 +1566,34 @@
         <v>3500</v>
       </c>
       <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C44" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D44" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B45" s="1">
         <v>200</v>
-      </c>
-      <c r="C44" t="s">
-        <v>12</v>
-      </c>
-      <c r="D44">
-        <v>99999</v>
-      </c>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="1">
-        <v>3600</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
@@ -1581,16 +1605,16 @@
     </row>
     <row r="46" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46" s="1">
-        <v>4600</v>
+        <v>3600</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>92</v>
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>99999</v>
       </c>
       <c r="E46" s="1"/>
     </row>
@@ -1602,10 +1626,10 @@
         <v>4600</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E47" s="1"/>
     </row>
@@ -1617,22 +1641,25 @@
         <v>4600</v>
       </c>
       <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="1">
+        <v>4600</v>
+      </c>
+      <c r="C49" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="1">
-        <v>150</v>
-      </c>
-      <c r="C49" t="s">
-        <v>5</v>
       </c>
       <c r="E49" s="1"/>
     </row>
@@ -1644,7 +1671,7 @@
         <v>150</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E50" s="1"/>
     </row>
@@ -1656,7 +1683,7 @@
         <v>150</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E51" s="1"/>
     </row>
@@ -1668,11 +1695,11 @@
         <v>150</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>31</v>
       </c>
@@ -1680,26 +1707,23 @@
         <v>150</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="1">
-        <v>2700</v>
+        <v>150</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>95</v>
+        <v>6</v>
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>32</v>
       </c>
@@ -1707,34 +1731,34 @@
         <v>2700</v>
       </c>
       <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2700</v>
+      </c>
+      <c r="C56" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B56" s="1">
-        <v>2000</v>
-      </c>
-      <c r="C56" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56">
-        <v>99999</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B57" s="1">
-        <v>2100</v>
+        <v>2000</v>
       </c>
       <c r="C57" t="s">
         <v>12</v>
@@ -1746,46 +1770,46 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="B58" s="1">
+        <v>2100</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58">
+        <v>99999</v>
+      </c>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" s="1">
         <v>5600</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59">
-        <v>2600</v>
-      </c>
-      <c r="C59" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59">
-        <v>99999</v>
+      <c r="D59" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B60" s="1">
-        <v>1100</v>
+        <v>35</v>
+      </c>
+      <c r="B60">
+        <v>2600</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>97</v>
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>99999</v>
       </c>
       <c r="E60" s="1"/>
     </row>
@@ -1797,10 +1821,10 @@
         <v>1100</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E61" s="1"/>
     </row>
@@ -1812,10 +1836,10 @@
         <v>1100</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E62" s="1"/>
     </row>
@@ -1827,34 +1851,34 @@
         <v>1100</v>
       </c>
       <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1100</v>
+      </c>
+      <c r="C64" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D64" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B64" s="1">
-        <v>3300</v>
-      </c>
-      <c r="C64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64">
-        <v>99999</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B65" s="1">
-        <v>5100</v>
+        <v>3300</v>
       </c>
       <c r="C65" t="s">
         <v>12</v>
@@ -1866,10 +1890,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B66" s="1">
-        <v>2800</v>
+        <v>5100</v>
       </c>
       <c r="C66" t="s">
         <v>12</v>
@@ -1879,12 +1903,12 @@
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B67" s="1">
-        <v>5200</v>
+        <v>2800</v>
       </c>
       <c r="C67" t="s">
         <v>12</v>
@@ -1894,12 +1918,12 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B68" s="1">
-        <v>4800</v>
+        <v>5200</v>
       </c>
       <c r="C68" t="s">
         <v>12</v>
@@ -1909,12 +1933,12 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>143</v>
+        <v>41</v>
       </c>
       <c r="B69" s="1">
-        <v>5300</v>
+        <v>4800</v>
       </c>
       <c r="C69" t="s">
         <v>12</v>
@@ -1926,10 +1950,10 @@
     </row>
     <row r="70" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="B70" s="1">
-        <v>4900</v>
+        <v>5300</v>
       </c>
       <c r="C70" t="s">
         <v>12</v>
@@ -1939,12 +1963,12 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B71" s="1">
-        <v>4100</v>
+        <v>4900</v>
       </c>
       <c r="C71" t="s">
         <v>12</v>
@@ -1956,10 +1980,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B72" s="1">
-        <v>5000</v>
+        <v>4100</v>
       </c>
       <c r="C72" t="s">
         <v>12</v>
@@ -1971,10 +1995,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="1">
-        <v>4500</v>
+        <v>5000</v>
       </c>
       <c r="C73" t="s">
         <v>12</v>
@@ -1986,10 +2010,10 @@
     </row>
     <row r="74" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B74" s="1">
-        <v>3400</v>
+        <v>4500</v>
       </c>
       <c r="C74" t="s">
         <v>12</v>
@@ -2001,13 +2025,13 @@
     </row>
     <row r="75" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B75" s="1">
-        <v>1200</v>
+        <v>3400</v>
       </c>
       <c r="C75" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>101</v>
@@ -2016,13 +2040,13 @@
     </row>
     <row r="76" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B76" s="1">
-        <v>1200</v>
+        <v>3400</v>
       </c>
       <c r="C76" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>102</v>
@@ -2031,13 +2055,13 @@
     </row>
     <row r="77" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B77" s="1">
-        <v>1200</v>
+        <v>3400</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>103</v>
@@ -2046,13 +2070,13 @@
     </row>
     <row r="78" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B78" s="1">
-        <v>1200</v>
+        <v>3400</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>104</v>
@@ -2061,73 +2085,73 @@
     </row>
     <row r="79" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B79" s="1">
-        <v>1400</v>
+        <v>3400</v>
       </c>
       <c r="C79" t="s">
-        <v>48</v>
-      </c>
-      <c r="D79" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>105</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B80" s="1">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="C80" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>106</v>
       </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B81" s="1">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="C81" t="s">
-        <v>8</v>
-      </c>
-      <c r="D81" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="5" t="s">
         <v>107</v>
       </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B82" s="1">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="C82" t="s">
-        <v>15</v>
-      </c>
-      <c r="D82" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B83" s="1">
-        <v>3900</v>
+        <v>1200</v>
       </c>
       <c r="C83" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>109</v>
@@ -2136,88 +2160,88 @@
     </row>
     <row r="84" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B84" s="1">
-        <v>3900</v>
+        <v>1400</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
-      </c>
-      <c r="D84" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D84" s="7" t="s">
         <v>110</v>
       </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B85" s="1">
-        <v>3900</v>
+        <v>1400</v>
       </c>
       <c r="C85" t="s">
-        <v>15</v>
-      </c>
-      <c r="D85" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="7" t="s">
         <v>111</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B86" s="1">
-        <v>3900</v>
+        <v>1400</v>
       </c>
       <c r="C86" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="7" t="s">
         <v>112</v>
       </c>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B87" s="1">
-        <v>3800</v>
+        <v>1400</v>
       </c>
       <c r="C87" t="s">
-        <v>5</v>
-      </c>
-      <c r="D87" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B88" s="1">
-        <v>3800</v>
+        <v>3900</v>
       </c>
       <c r="C88" t="s">
-        <v>15</v>
-      </c>
-      <c r="D88" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>114</v>
       </c>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B89" s="1">
-        <v>1300</v>
+        <v>3900</v>
       </c>
       <c r="C89" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>115</v>
@@ -2226,13 +2250,13 @@
     </row>
     <row r="90" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B90" s="1">
-        <v>1300</v>
+        <v>3900</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>116</v>
@@ -2241,13 +2265,13 @@
     </row>
     <row r="91" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B91" s="1">
-        <v>1300</v>
+        <v>3900</v>
       </c>
       <c r="C91" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>117</v>
@@ -2256,88 +2280,88 @@
     </row>
     <row r="92" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B92" s="1">
-        <v>1300</v>
+        <v>3800</v>
       </c>
       <c r="C92" t="s">
-        <v>15</v>
-      </c>
-      <c r="D92" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="7" t="s">
         <v>118</v>
       </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B93" s="1">
-        <v>1300</v>
+        <v>3800</v>
       </c>
       <c r="C93" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93" s="7" t="s">
         <v>119</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B94" s="1">
-        <v>2500</v>
+        <v>1300</v>
       </c>
       <c r="C94" t="s">
-        <v>48</v>
-      </c>
-      <c r="D94" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>120</v>
       </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B95" s="1">
-        <v>2500</v>
+        <v>1300</v>
       </c>
       <c r="C95" t="s">
-        <v>5</v>
-      </c>
-      <c r="D95" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="5" t="s">
         <v>121</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B96" s="1">
-        <v>2500</v>
+        <v>1300</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>122</v>
       </c>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B97" s="1">
-        <v>6000</v>
+        <v>1300</v>
       </c>
       <c r="C97" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>123</v>
@@ -2346,193 +2370,193 @@
     </row>
     <row r="98" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B98" s="1">
-        <v>6000</v>
+        <v>1300</v>
       </c>
       <c r="C98" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>124</v>
       </c>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B99" s="1">
-        <v>6000</v>
+        <v>2500</v>
       </c>
       <c r="C99" t="s">
-        <v>15</v>
-      </c>
-      <c r="D99" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D99" s="10" t="s">
         <v>125</v>
       </c>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
-        <v>146</v>
+        <v>53</v>
       </c>
       <c r="B100" s="1">
-        <v>5400</v>
+        <v>2500</v>
       </c>
       <c r="C100" t="s">
-        <v>12</v>
-      </c>
-      <c r="D100" s="5">
-        <v>99999</v>
+        <v>5</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B101" s="1">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="C101" t="s">
-        <v>5</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>128</v>
+        <v>8</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>127</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B102" s="1">
-        <v>1000</v>
+        <v>6000</v>
       </c>
       <c r="C102" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B103" s="1">
-        <v>1000</v>
+        <v>6000</v>
       </c>
       <c r="C103" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B104" s="1">
-        <v>1900</v>
+        <v>6000</v>
       </c>
       <c r="C104" t="s">
-        <v>5</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>129</v>
+        <v>15</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="B105" s="1">
-        <v>1900</v>
+        <v>5400</v>
       </c>
       <c r="C105" t="s">
-        <v>8</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>130</v>
+        <v>12</v>
+      </c>
+      <c r="D105" s="5">
+        <v>99999</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B106" s="1">
-        <v>1900</v>
+        <v>1000</v>
       </c>
       <c r="C106" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B107" s="1">
-        <v>1900</v>
+        <v>1000</v>
       </c>
       <c r="C107" t="s">
         <v>15</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B108" s="1">
-        <v>1900</v>
+        <v>1000</v>
       </c>
       <c r="C108" t="s">
         <v>6</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B109" s="1">
-        <v>4000</v>
+        <v>1900</v>
       </c>
       <c r="C109" t="s">
         <v>5</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D109" s="4" t="s">
         <v>134</v>
       </c>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B110" s="1">
-        <v>4000</v>
+        <v>1900</v>
       </c>
       <c r="C110" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>135</v>
@@ -2541,13 +2565,13 @@
     </row>
     <row r="111" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B111" s="1">
-        <v>4000</v>
+        <v>1900</v>
       </c>
       <c r="C111" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>136</v>
@@ -2556,55 +2580,55 @@
     </row>
     <row r="112" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B112" s="1">
-        <v>6500</v>
+        <v>1900</v>
       </c>
       <c r="C112" t="s">
-        <v>48</v>
-      </c>
-      <c r="D112" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112" s="5" t="s">
         <v>137</v>
       </c>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B113" s="1">
-        <v>6500</v>
+        <v>1900</v>
       </c>
       <c r="C113" t="s">
-        <v>5</v>
-      </c>
-      <c r="D113" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="5" t="s">
         <v>138</v>
       </c>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B114" s="1">
-        <v>6500</v>
+        <v>4000</v>
       </c>
       <c r="C114" t="s">
-        <v>8</v>
-      </c>
-      <c r="D114" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" s="5" t="s">
         <v>139</v>
       </c>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B115" s="1">
-        <v>6500</v>
+        <v>4000</v>
       </c>
       <c r="C115" t="s">
         <v>9</v>
@@ -2616,20 +2640,20 @@
     </row>
     <row r="116" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B116" s="1">
-        <v>6500</v>
-      </c>
-      <c r="C116" s="9" t="s">
+        <v>4000</v>
+      </c>
+      <c r="C116" t="s">
         <v>15</v>
       </c>
-      <c r="D116" s="11" t="s">
+      <c r="D116" s="5" t="s">
         <v>141</v>
       </c>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>58</v>
       </c>
@@ -2637,208 +2661,316 @@
         <v>6500</v>
       </c>
       <c r="C117" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D117" s="11" t="s">
         <v>142</v>
       </c>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B118" s="1">
-        <v>4400</v>
+        <v>6500</v>
       </c>
       <c r="C118" t="s">
         <v>5</v>
       </c>
-      <c r="D118" s="11"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D118" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B119" s="1">
-        <v>4400</v>
+        <v>6500</v>
       </c>
       <c r="C119" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D119" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E119" s="1"/>
+    </row>
+    <row r="120" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B120" s="1">
-        <v>4400</v>
+        <v>6500</v>
       </c>
       <c r="C120" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D120" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E120" s="1"/>
+    </row>
+    <row r="121" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B121" s="1">
-        <v>4400</v>
-      </c>
-      <c r="C121" t="s">
+        <v>6500</v>
+      </c>
+      <c r="C121" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D121" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E121" s="1"/>
+    </row>
+    <row r="122" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B122" s="1">
-        <v>4400</v>
+        <v>6500</v>
       </c>
       <c r="C122" t="s">
         <v>6</v>
       </c>
+      <c r="D122" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E122" s="1"/>
+    </row>
+    <row r="123" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B123" s="1">
+        <v>5800</v>
+      </c>
+      <c r="C123" t="s">
+        <v>12</v>
+      </c>
+      <c r="D123" s="5">
+        <v>99999</v>
+      </c>
+      <c r="E123" s="1"/>
+    </row>
+    <row r="124" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B124" s="1">
+        <v>4400</v>
+      </c>
+      <c r="C124" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" s="11"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B125" s="1">
+        <v>4400</v>
+      </c>
+      <c r="C125" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B126" s="1">
+        <v>4400</v>
+      </c>
+      <c r="C126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B127" s="1">
+        <v>4400</v>
+      </c>
+      <c r="C127" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B128" s="1">
+        <v>4400</v>
+      </c>
+      <c r="C128" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>154</v>
+      </c>
+      <c r="B129" s="1">
+        <v>5900</v>
+      </c>
+      <c r="C129" t="s">
+        <v>12</v>
+      </c>
+      <c r="D129" s="5">
+        <v>99999</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="A17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="A18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="A19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="A20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="A21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="A32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="A35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="A39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="A42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="A43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="A44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="A45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="A46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="A47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="A48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="A49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="A50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="A51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="A52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="A53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="A54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="A55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="A56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="A57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="A59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="A60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="A61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="A62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="A63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="A64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="A65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="A66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="A67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="A68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="A95" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="A96" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="A97" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="A98" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="A99" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="A101" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="A102" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="A103" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="A104" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="A105" r:id="rId76" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="A106" r:id="rId77" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="A107" r:id="rId78" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="A108" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="A109" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="A110" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="A111" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="A112" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="A113" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="A114" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="A116" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="A117" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="A118" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="A119" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="A120" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="A121" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="A122" r:id="rId92" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="D2" r:id="rId93" display="http://sabose.cu/" xr:uid="{47EDC6A2-E374-4384-83BF-1151296A8B80}"/>
-    <hyperlink ref="D21" r:id="rId94" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{8191FBBF-8854-4C0A-8B84-E84F0CC1A943}"/>
-    <hyperlink ref="D24" r:id="rId95" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{BBD40848-FBCD-4DBE-ADBF-830C639AC43C}"/>
-    <hyperlink ref="D23" r:id="rId96" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{E347D519-C1BE-4E2F-9DE2-4F876CAA1896}"/>
-    <hyperlink ref="D22" r:id="rId97" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{099130F4-96CB-41A1-AF6B-E959DE9F4517}"/>
-    <hyperlink ref="D37" r:id="rId98" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTMwMDAmb3JnSWQ9MTQ2NzU0&amp;person_id=22297698&amp;forPersonCustId=3000" xr:uid="{850A56CE-02C6-4335-82D5-BC8FCA19D520}"/>
-    <hyperlink ref="D40" r:id="rId99" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=21687687&amp;forPersonCustId=3000" xr:uid="{2E221ED3-44BB-4C33-B120-4A5DC7FC4D0C}"/>
-    <hyperlink ref="D41" r:id="rId100" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{90032F47-9BAC-4D8F-9DEB-338BF29E04F2}"/>
-    <hyperlink ref="D42" r:id="rId101" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{1D2F84AA-1DE0-4251-9DAE-1EF798CFEFBC}"/>
-    <hyperlink ref="D43" r:id="rId102" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{AD4A5868-800F-42DC-8BEC-9F2A06319281}"/>
-    <hyperlink ref="D79" r:id="rId103" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=6929346&amp;forPersonCustId=47" xr:uid="{1EBA4DAD-A644-4D69-939A-195D56E5D254}"/>
-    <hyperlink ref="D80" r:id="rId104" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36889637&amp;forPersonCustId=1400" xr:uid="{AE6AD973-8B2E-45FA-B623-EA01EBEE0AFD}"/>
-    <hyperlink ref="D81" r:id="rId105" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=22433553&amp;forPersonCustId=1400" xr:uid="{962BF6F0-F8E6-4D8B-B56F-CDB12A596BA0}"/>
-    <hyperlink ref="D87" r:id="rId106" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{7FD4B6CF-752F-4666-818B-8BA80FC216F5}"/>
-    <hyperlink ref="D88" r:id="rId107" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{30966F6F-B77C-4914-AB8D-A15DBD0329F5}"/>
-    <hyperlink ref="D104" r:id="rId108" display="http://puchakraborty.cm/" xr:uid="{FB84B2F6-939B-44E5-95B2-C963662FBD0C}"/>
-    <hyperlink ref="A115" r:id="rId109" xr:uid="{2D237A29-BE80-4D01-9992-C2BEB4FB6FC3}"/>
-    <hyperlink ref="A94" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="A93" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="A92" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="A91" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="A90" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="A89" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="A88" r:id="rId116" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="A87" r:id="rId117" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="A86" r:id="rId118" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="A85" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="A84" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="A83" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="A82" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="A81" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="A80" r:id="rId124" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="A79" r:id="rId125" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="A78" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="A77" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="A76" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="A75" r:id="rId129" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="A74" r:id="rId130" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="A73" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="A72" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="A71" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="A70" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="A43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="A45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="A54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="A55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="A56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="A57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="A58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="A60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="A61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="A62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="A63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="A64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="A65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="A66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="A67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="A68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="A69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="A100" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="A101" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="A102" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="A103" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="A104" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="A106" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="A107" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="A108" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="A109" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="A110" r:id="rId76" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="A111" r:id="rId77" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="A112" r:id="rId78" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="A113" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="A114" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="A115" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="A116" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="A117" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="A118" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="A119" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="A121" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="A122" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="A124" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="A125" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="A126" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="A127" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="A128" r:id="rId92" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="D3" r:id="rId93" display="http://sabose.cu/" xr:uid="{47EDC6A2-E374-4384-83BF-1151296A8B80}"/>
+    <hyperlink ref="D22" r:id="rId94" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{8191FBBF-8854-4C0A-8B84-E84F0CC1A943}"/>
+    <hyperlink ref="D25" r:id="rId95" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{BBD40848-FBCD-4DBE-ADBF-830C639AC43C}"/>
+    <hyperlink ref="D24" r:id="rId96" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{E347D519-C1BE-4E2F-9DE2-4F876CAA1896}"/>
+    <hyperlink ref="D23" r:id="rId97" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{099130F4-96CB-41A1-AF6B-E959DE9F4517}"/>
+    <hyperlink ref="D38" r:id="rId98" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTMwMDAmb3JnSWQ9MTQ2NzU0&amp;person_id=22297698&amp;forPersonCustId=3000" xr:uid="{850A56CE-02C6-4335-82D5-BC8FCA19D520}"/>
+    <hyperlink ref="D41" r:id="rId99" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=21687687&amp;forPersonCustId=3000" xr:uid="{2E221ED3-44BB-4C33-B120-4A5DC7FC4D0C}"/>
+    <hyperlink ref="D42" r:id="rId100" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{90032F47-9BAC-4D8F-9DEB-338BF29E04F2}"/>
+    <hyperlink ref="D43" r:id="rId101" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{1D2F84AA-1DE0-4251-9DAE-1EF798CFEFBC}"/>
+    <hyperlink ref="D44" r:id="rId102" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{AD4A5868-800F-42DC-8BEC-9F2A06319281}"/>
+    <hyperlink ref="D84" r:id="rId103" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=6929346&amp;forPersonCustId=47" xr:uid="{1EBA4DAD-A644-4D69-939A-195D56E5D254}"/>
+    <hyperlink ref="D85" r:id="rId104" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36889637&amp;forPersonCustId=1400" xr:uid="{AE6AD973-8B2E-45FA-B623-EA01EBEE0AFD}"/>
+    <hyperlink ref="D86" r:id="rId105" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=22433553&amp;forPersonCustId=1400" xr:uid="{962BF6F0-F8E6-4D8B-B56F-CDB12A596BA0}"/>
+    <hyperlink ref="D92" r:id="rId106" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{7FD4B6CF-752F-4666-818B-8BA80FC216F5}"/>
+    <hyperlink ref="D93" r:id="rId107" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{30966F6F-B77C-4914-AB8D-A15DBD0329F5}"/>
+    <hyperlink ref="D109" r:id="rId108" display="http://puchakraborty.cm/" xr:uid="{FB84B2F6-939B-44E5-95B2-C963662FBD0C}"/>
+    <hyperlink ref="A120" r:id="rId109" xr:uid="{2D237A29-BE80-4D01-9992-C2BEB4FB6FC3}"/>
+    <hyperlink ref="A99" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="A98" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="A97" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="A96" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="A95" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="A94" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="A93" r:id="rId116" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="A92" r:id="rId117" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="A91" r:id="rId118" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="A90" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="A89" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="A88" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="A87" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="A86" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="A85" r:id="rId124" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A84" r:id="rId125" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="A83" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="A82" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="A81" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="A80" r:id="rId129" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="A79" r:id="rId130" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="A78" r:id="rId131" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="A77" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A76" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="A75" r:id="rId134" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="A74" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="A73" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="A72" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A71" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId135"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId139"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Removed Anthenm Regional supports
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC17FA3F-FAC7-4F3F-A0E4-7FE6007C0ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6098DFD-340B-4D6C-A1C3-0130D194E19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-4620" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="154">
   <si>
     <t>Customer Name</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>anthm_kjacobo</t>
-  </si>
-  <si>
-    <t>anthm_mfierro</t>
   </si>
   <si>
     <t>btp_agodinez</t>
@@ -927,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -957,7 +954,7 @@
     </row>
     <row r="2" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2">
         <v>99999</v>
@@ -1071,34 +1068,34 @@
         <v>3700</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>3700</v>
+        <v>2200</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>64</v>
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>99999</v>
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>2200</v>
+        <v>4200</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1110,16 +1107,16 @@
     </row>
     <row r="13" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>4200</v>
+        <v>1600</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>99999</v>
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -1131,7 +1128,7 @@
         <v>1600</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>65</v>
@@ -1146,7 +1143,7 @@
         <v>1600</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>66</v>
@@ -1161,7 +1158,7 @@
         <v>1600</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>67</v>
@@ -1176,7 +1173,7 @@
         <v>1600</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>68</v>
@@ -1185,31 +1182,31 @@
     </row>
     <row r="18" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>1600</v>
+        <v>4700</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>69</v>
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>99999</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>4700</v>
+        <v>3200</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19">
-        <v>99999</v>
+        <v>5</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -1221,7 +1218,7 @@
         <v>3200</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>70</v>
@@ -1236,22 +1233,22 @@
         <v>3200</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>71</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1">
-        <v>3200</v>
+        <v>3100</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>72</v>
@@ -1266,7 +1263,7 @@
         <v>3100</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>73</v>
@@ -1281,7 +1278,7 @@
         <v>3100</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>74</v>
@@ -1290,15 +1287,15 @@
     </row>
     <row r="25" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1">
-        <v>3100</v>
+        <v>1700</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E25" s="1"/>
@@ -1311,7 +1308,7 @@
         <v>1700</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>76</v>
@@ -1326,25 +1323,25 @@
         <v>1700</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>77</v>
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B28" s="1">
-        <v>1700</v>
+        <v>2900</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E28" s="1"/>
     </row>
@@ -1356,14 +1353,14 @@
         <v>2900</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -1371,25 +1368,25 @@
         <v>2900</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1">
-        <v>2900</v>
+        <v>1800</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="E31" s="1"/>
     </row>
@@ -1401,7 +1398,7 @@
         <v>1800</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>79</v>
@@ -1416,7 +1413,7 @@
         <v>1800</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>80</v>
@@ -1431,7 +1428,7 @@
         <v>1800</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>81</v>
@@ -1440,15 +1437,15 @@
     </row>
     <row r="35" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1">
-        <v>1800</v>
+        <v>4300</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>82</v>
       </c>
       <c r="E35" s="1"/>
@@ -1461,7 +1458,7 @@
         <v>4300</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>83</v>
@@ -1470,15 +1467,15 @@
     </row>
     <row r="37" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B37" s="1">
-        <v>4300</v>
+        <v>3000</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>84</v>
       </c>
       <c r="E37" s="1"/>
@@ -1491,9 +1488,9 @@
         <v>3000</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>85</v>
       </c>
       <c r="E38" s="1"/>
@@ -1506,9 +1503,9 @@
         <v>3000</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>86</v>
       </c>
       <c r="E39" s="1"/>
@@ -1521,22 +1518,22 @@
         <v>3000</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B41" s="1">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>88</v>
@@ -1551,7 +1548,7 @@
         <v>3500</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>89</v>
@@ -1566,34 +1563,34 @@
         <v>3500</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>90</v>
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B44" s="1">
-        <v>3500</v>
+        <v>200</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>91</v>
+        <v>12</v>
+      </c>
+      <c r="D44">
+        <v>99999</v>
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B45" s="1">
-        <v>200</v>
+        <v>3600</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
@@ -1605,16 +1602,16 @@
     </row>
     <row r="46" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B46" s="1">
-        <v>3600</v>
+        <v>4600</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46">
-        <v>99999</v>
+        <v>5</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="E46" s="1"/>
     </row>
@@ -1626,7 +1623,7 @@
         <v>4600</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>92</v>
@@ -1641,25 +1638,22 @@
         <v>4600</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B49" s="1">
-        <v>4600</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="E49" s="1"/>
     </row>
@@ -1671,7 +1665,7 @@
         <v>150</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E50" s="1"/>
     </row>
@@ -1683,7 +1677,7 @@
         <v>150</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E51" s="1"/>
     </row>
@@ -1695,11 +1689,11 @@
         <v>150</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>31</v>
       </c>
@@ -1707,23 +1701,26 @@
         <v>150</v>
       </c>
       <c r="C53" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B54" s="1">
-        <v>150</v>
+        <v>2700</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>32</v>
       </c>
@@ -1731,34 +1728,34 @@
         <v>2700</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>95</v>
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B56" s="1">
-        <v>2700</v>
+        <v>2000</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>96</v>
+        <v>12</v>
+      </c>
+      <c r="D56">
+        <v>99999</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B57" s="1">
-        <v>2000</v>
+        <v>2100</v>
       </c>
       <c r="C57" t="s">
         <v>12</v>
@@ -1770,46 +1767,46 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>34</v>
+        <v>148</v>
       </c>
       <c r="B58" s="1">
-        <v>2100</v>
+        <v>5600</v>
       </c>
       <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59">
+        <v>2600</v>
+      </c>
+      <c r="C59" t="s">
         <v>12</v>
       </c>
-      <c r="D58">
+      <c r="D59">
         <v>99999</v>
-      </c>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B59" s="1">
-        <v>5600</v>
-      </c>
-      <c r="C59" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>150</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B60">
-        <v>2600</v>
+        <v>36</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1100</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60">
-        <v>99999</v>
+        <v>5</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="E60" s="1"/>
     </row>
@@ -1821,7 +1818,7 @@
         <v>1100</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>97</v>
@@ -1836,7 +1833,7 @@
         <v>1100</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>98</v>
@@ -1851,34 +1848,34 @@
         <v>1100</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>99</v>
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B64" s="1">
-        <v>1100</v>
+        <v>3300</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>100</v>
+        <v>12</v>
+      </c>
+      <c r="D64">
+        <v>99999</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B65" s="1">
-        <v>3300</v>
+        <v>5100</v>
       </c>
       <c r="C65" t="s">
         <v>12</v>
@@ -1890,10 +1887,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B66" s="1">
-        <v>5100</v>
+        <v>2800</v>
       </c>
       <c r="C66" t="s">
         <v>12</v>
@@ -1903,12 +1900,12 @@
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B67" s="1">
-        <v>2800</v>
+        <v>5200</v>
       </c>
       <c r="C67" t="s">
         <v>12</v>
@@ -1918,12 +1915,12 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B68" s="1">
-        <v>5200</v>
+        <v>4800</v>
       </c>
       <c r="C68" t="s">
         <v>12</v>
@@ -1933,12 +1930,12 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="B69" s="1">
-        <v>4800</v>
+        <v>5300</v>
       </c>
       <c r="C69" t="s">
         <v>12</v>
@@ -1950,10 +1947,10 @@
     </row>
     <row r="70" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
       <c r="B70" s="1">
-        <v>5300</v>
+        <v>4900</v>
       </c>
       <c r="C70" t="s">
         <v>12</v>
@@ -1963,12 +1960,12 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B71" s="1">
-        <v>4900</v>
+        <v>4100</v>
       </c>
       <c r="C71" t="s">
         <v>12</v>
@@ -1980,10 +1977,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B72" s="1">
-        <v>4100</v>
+        <v>5000</v>
       </c>
       <c r="C72" t="s">
         <v>12</v>
@@ -1993,12 +1990,12 @@
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B73" s="1">
-        <v>5000</v>
+        <v>4500</v>
       </c>
       <c r="C73" t="s">
         <v>12</v>
@@ -2010,16 +2007,16 @@
     </row>
     <row r="74" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B74" s="1">
-        <v>4500</v>
+        <v>3400</v>
       </c>
       <c r="C74" t="s">
-        <v>12</v>
-      </c>
-      <c r="D74">
-        <v>99999</v>
+        <v>5</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="E74" s="1"/>
     </row>
@@ -2031,7 +2028,7 @@
         <v>3400</v>
       </c>
       <c r="C75" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>101</v>
@@ -2046,7 +2043,7 @@
         <v>3400</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>102</v>
@@ -2061,7 +2058,7 @@
         <v>3400</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>103</v>
@@ -2076,7 +2073,7 @@
         <v>3400</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>104</v>
@@ -2085,13 +2082,13 @@
     </row>
     <row r="79" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B79" s="1">
-        <v>3400</v>
+        <v>1200</v>
       </c>
       <c r="C79" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>105</v>
@@ -2106,7 +2103,7 @@
         <v>1200</v>
       </c>
       <c r="C80" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>106</v>
@@ -2121,7 +2118,7 @@
         <v>1200</v>
       </c>
       <c r="C81" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>107</v>
@@ -2136,7 +2133,7 @@
         <v>1200</v>
       </c>
       <c r="C82" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>108</v>
@@ -2145,15 +2142,15 @@
     </row>
     <row r="83" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B83" s="1">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="C83" t="s">
-        <v>9</v>
-      </c>
-      <c r="D83" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D83" s="7" t="s">
         <v>109</v>
       </c>
       <c r="E83" s="1"/>
@@ -2166,7 +2163,7 @@
         <v>1400</v>
       </c>
       <c r="C84" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>110</v>
@@ -2181,7 +2178,7 @@
         <v>1400</v>
       </c>
       <c r="C85" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>111</v>
@@ -2196,24 +2193,24 @@
         <v>1400</v>
       </c>
       <c r="C86" t="s">
-        <v>8</v>
-      </c>
-      <c r="D86" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="6" t="s">
         <v>112</v>
       </c>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B87" s="1">
-        <v>1400</v>
+        <v>3900</v>
       </c>
       <c r="C87" t="s">
-        <v>15</v>
-      </c>
-      <c r="D87" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>113</v>
       </c>
       <c r="E87" s="1"/>
@@ -2226,7 +2223,7 @@
         <v>3900</v>
       </c>
       <c r="C88" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>114</v>
@@ -2241,7 +2238,7 @@
         <v>3900</v>
       </c>
       <c r="C89" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>115</v>
@@ -2256,7 +2253,7 @@
         <v>3900</v>
       </c>
       <c r="C90" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>116</v>
@@ -2265,15 +2262,15 @@
     </row>
     <row r="91" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B91" s="1">
-        <v>3900</v>
+        <v>3800</v>
       </c>
       <c r="C91" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="7" t="s">
         <v>117</v>
       </c>
       <c r="E91" s="1"/>
@@ -2286,7 +2283,7 @@
         <v>3800</v>
       </c>
       <c r="C92" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>118</v>
@@ -2295,15 +2292,15 @@
     </row>
     <row r="93" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B93" s="1">
-        <v>3800</v>
+        <v>1300</v>
       </c>
       <c r="C93" t="s">
-        <v>15</v>
-      </c>
-      <c r="D93" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>119</v>
       </c>
       <c r="E93" s="1"/>
@@ -2316,7 +2313,7 @@
         <v>1300</v>
       </c>
       <c r="C94" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>120</v>
@@ -2331,7 +2328,7 @@
         <v>1300</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>121</v>
@@ -2346,7 +2343,7 @@
         <v>1300</v>
       </c>
       <c r="C96" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>122</v>
@@ -2361,7 +2358,7 @@
         <v>1300</v>
       </c>
       <c r="C97" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>123</v>
@@ -2370,20 +2367,20 @@
     </row>
     <row r="98" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B98" s="1">
-        <v>1300</v>
+        <v>2500</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D98" s="10" t="s">
         <v>124</v>
       </c>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -2391,14 +2388,14 @@
         <v>2500</v>
       </c>
       <c r="C99" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D99" s="10" t="s">
         <v>125</v>
       </c>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>53</v>
       </c>
@@ -2406,24 +2403,24 @@
         <v>2500</v>
       </c>
       <c r="C100" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>126</v>
       </c>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B101" s="1">
-        <v>2500</v>
+        <v>6000</v>
       </c>
       <c r="C101" t="s">
-        <v>8</v>
-      </c>
-      <c r="D101" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>127</v>
       </c>
       <c r="E101" s="1"/>
@@ -2436,7 +2433,7 @@
         <v>6000</v>
       </c>
       <c r="C102" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>128</v>
@@ -2451,40 +2448,40 @@
         <v>6000</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>129</v>
       </c>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="B104" s="1">
-        <v>6000</v>
+        <v>5400</v>
       </c>
       <c r="C104" t="s">
-        <v>15</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>130</v>
+        <v>12</v>
+      </c>
+      <c r="D104" s="5">
+        <v>99999</v>
       </c>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="B105" s="1">
-        <v>5400</v>
+        <v>1000</v>
       </c>
       <c r="C105" t="s">
-        <v>12</v>
-      </c>
-      <c r="D105" s="5">
-        <v>99999</v>
+        <v>5</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="E105" s="1"/>
     </row>
@@ -2496,10 +2493,10 @@
         <v>1000</v>
       </c>
       <c r="C106" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E106" s="1"/>
     </row>
@@ -2511,7 +2508,7 @@
         <v>1000</v>
       </c>
       <c r="C107" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>131</v>
@@ -2520,16 +2517,16 @@
     </row>
     <row r="108" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B108" s="1">
-        <v>1000</v>
+        <v>1900</v>
       </c>
       <c r="C108" t="s">
-        <v>6</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>132</v>
+        <v>5</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="E108" s="1"/>
     </row>
@@ -2541,9 +2538,9 @@
         <v>1900</v>
       </c>
       <c r="C109" t="s">
-        <v>5</v>
-      </c>
-      <c r="D109" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" s="5" t="s">
         <v>134</v>
       </c>
       <c r="E109" s="1"/>
@@ -2556,7 +2553,7 @@
         <v>1900</v>
       </c>
       <c r="C110" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>135</v>
@@ -2571,7 +2568,7 @@
         <v>1900</v>
       </c>
       <c r="C111" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>136</v>
@@ -2586,7 +2583,7 @@
         <v>1900</v>
       </c>
       <c r="C112" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>137</v>
@@ -2595,13 +2592,13 @@
     </row>
     <row r="113" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B113" s="1">
-        <v>1900</v>
+        <v>4000</v>
       </c>
       <c r="C113" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>138</v>
@@ -2616,7 +2613,7 @@
         <v>4000</v>
       </c>
       <c r="C114" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>139</v>
@@ -2631,7 +2628,7 @@
         <v>4000</v>
       </c>
       <c r="C115" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>140</v>
@@ -2640,20 +2637,20 @@
     </row>
     <row r="116" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B116" s="1">
-        <v>4000</v>
+        <v>6500</v>
       </c>
       <c r="C116" t="s">
-        <v>15</v>
-      </c>
-      <c r="D116" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D116" s="11" t="s">
         <v>141</v>
       </c>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>58</v>
       </c>
@@ -2661,14 +2658,14 @@
         <v>6500</v>
       </c>
       <c r="C117" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D117" s="11" t="s">
         <v>142</v>
       </c>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>58</v>
       </c>
@@ -2676,14 +2673,14 @@
         <v>6500</v>
       </c>
       <c r="C118" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D118" s="11" t="s">
         <v>143</v>
       </c>
       <c r="E118" s="1"/>
     </row>
-    <row r="119" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>58</v>
       </c>
@@ -2691,9 +2688,9 @@
         <v>6500</v>
       </c>
       <c r="C119" t="s">
-        <v>8</v>
-      </c>
-      <c r="D119" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" s="5" t="s">
         <v>144</v>
       </c>
       <c r="E119" s="1"/>
@@ -2705,60 +2702,57 @@
       <c r="B120" s="1">
         <v>6500</v>
       </c>
-      <c r="C120" t="s">
-        <v>9</v>
-      </c>
-      <c r="D120" s="5" t="s">
+      <c r="C120" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120" s="11" t="s">
         <v>145</v>
       </c>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B121" s="1">
         <v>6500</v>
       </c>
-      <c r="C121" s="9" t="s">
-        <v>15</v>
+      <c r="C121" t="s">
+        <v>6</v>
       </c>
       <c r="D121" s="11" t="s">
         <v>146</v>
       </c>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="B122" s="1">
-        <v>6500</v>
+        <v>5800</v>
       </c>
       <c r="C122" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122" s="11" t="s">
-        <v>147</v>
+        <v>12</v>
+      </c>
+      <c r="D122" s="5">
+        <v>99999</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>153</v>
+        <v>59</v>
       </c>
       <c r="B123" s="1">
-        <v>5800</v>
+        <v>4400</v>
       </c>
       <c r="C123" t="s">
-        <v>12</v>
-      </c>
-      <c r="D123" s="5">
-        <v>99999</v>
-      </c>
-      <c r="E123" s="1"/>
-    </row>
-    <row r="124" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D123" s="11"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>59</v>
       </c>
@@ -2766,9 +2760,8 @@
         <v>4400</v>
       </c>
       <c r="C124" t="s">
-        <v>5</v>
-      </c>
-      <c r="D124" s="11"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
@@ -2778,7 +2771,7 @@
         <v>4400</v>
       </c>
       <c r="C125" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -2789,10 +2782,10 @@
         <v>4400</v>
       </c>
       <c r="C126" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>59</v>
       </c>
@@ -2800,31 +2793,20 @@
         <v>4400</v>
       </c>
       <c r="C127" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="2" t="s">
-        <v>59</v>
+      <c r="A128" t="s">
+        <v>153</v>
       </c>
       <c r="B128" s="1">
-        <v>4400</v>
+        <v>5900</v>
       </c>
       <c r="C128" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>154</v>
-      </c>
-      <c r="B129" s="1">
-        <v>5900</v>
-      </c>
-      <c r="C129" t="s">
         <v>12</v>
       </c>
-      <c r="D129" s="5">
+      <c r="D128" s="5">
         <v>99999</v>
       </c>
     </row>
@@ -2837,140 +2819,139 @@
     <hyperlink ref="A7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="A8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="A9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="A18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="A19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="A20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="A21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="A22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="A33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="A36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="A40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="A43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="A44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="A45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="A46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="A47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="A48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="A49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="A50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="A51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="A52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="A53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="A54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="A55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="A56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="A57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="A58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="A60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="A61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="A62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="A63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="A64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="A65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="A66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="A67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="A68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="A69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="A100" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="A101" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="A102" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="A103" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="A104" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="A106" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="A107" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="A108" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="A109" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="A110" r:id="rId76" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="A111" r:id="rId77" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="A112" r:id="rId78" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="A113" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="A114" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="A115" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="A116" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="A117" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="A118" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="A119" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="A121" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="A122" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="A124" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="A125" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="A126" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="A127" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="A128" r:id="rId92" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="D3" r:id="rId93" display="http://sabose.cu/" xr:uid="{47EDC6A2-E374-4384-83BF-1151296A8B80}"/>
-    <hyperlink ref="D22" r:id="rId94" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{8191FBBF-8854-4C0A-8B84-E84F0CC1A943}"/>
-    <hyperlink ref="D25" r:id="rId95" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{BBD40848-FBCD-4DBE-ADBF-830C639AC43C}"/>
-    <hyperlink ref="D24" r:id="rId96" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{E347D519-C1BE-4E2F-9DE2-4F876CAA1896}"/>
-    <hyperlink ref="D23" r:id="rId97" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{099130F4-96CB-41A1-AF6B-E959DE9F4517}"/>
-    <hyperlink ref="D38" r:id="rId98" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTMwMDAmb3JnSWQ9MTQ2NzU0&amp;person_id=22297698&amp;forPersonCustId=3000" xr:uid="{850A56CE-02C6-4335-82D5-BC8FCA19D520}"/>
-    <hyperlink ref="D41" r:id="rId99" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=21687687&amp;forPersonCustId=3000" xr:uid="{2E221ED3-44BB-4C33-B120-4A5DC7FC4D0C}"/>
-    <hyperlink ref="D42" r:id="rId100" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{90032F47-9BAC-4D8F-9DEB-338BF29E04F2}"/>
-    <hyperlink ref="D43" r:id="rId101" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{1D2F84AA-1DE0-4251-9DAE-1EF798CFEFBC}"/>
-    <hyperlink ref="D44" r:id="rId102" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{AD4A5868-800F-42DC-8BEC-9F2A06319281}"/>
-    <hyperlink ref="D84" r:id="rId103" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=6929346&amp;forPersonCustId=47" xr:uid="{1EBA4DAD-A644-4D69-939A-195D56E5D254}"/>
-    <hyperlink ref="D85" r:id="rId104" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36889637&amp;forPersonCustId=1400" xr:uid="{AE6AD973-8B2E-45FA-B623-EA01EBEE0AFD}"/>
-    <hyperlink ref="D86" r:id="rId105" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=22433553&amp;forPersonCustId=1400" xr:uid="{962BF6F0-F8E6-4D8B-B56F-CDB12A596BA0}"/>
-    <hyperlink ref="D92" r:id="rId106" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{7FD4B6CF-752F-4666-818B-8BA80FC216F5}"/>
-    <hyperlink ref="D93" r:id="rId107" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{30966F6F-B77C-4914-AB8D-A15DBD0329F5}"/>
-    <hyperlink ref="D109" r:id="rId108" display="http://puchakraborty.cm/" xr:uid="{FB84B2F6-939B-44E5-95B2-C963662FBD0C}"/>
-    <hyperlink ref="A120" r:id="rId109" xr:uid="{2D237A29-BE80-4D01-9992-C2BEB4FB6FC3}"/>
-    <hyperlink ref="A99" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="A98" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="A97" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="A96" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="A95" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="A94" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="A93" r:id="rId116" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="A92" r:id="rId117" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="A91" r:id="rId118" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="A90" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="A89" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="A88" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="A87" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="A86" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="A85" r:id="rId124" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="A84" r:id="rId125" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="A83" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="A82" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="A81" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="A80" r:id="rId129" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="A79" r:id="rId130" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="A78" r:id="rId131" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="A77" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="A76" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="A75" r:id="rId134" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="A74" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="A73" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="A72" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="A71" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="A42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="A44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="A53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="A54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="A55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="A56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="A57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="A59" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="A60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="A61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="A62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="A63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="A64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="A65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="A66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="A67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="A68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="A99" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="A100" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="A101" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="A102" r:id="rId69" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="A103" r:id="rId70" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="A105" r:id="rId71" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="A106" r:id="rId72" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="A107" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="A108" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="A109" r:id="rId75" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="A110" r:id="rId76" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="A111" r:id="rId77" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="A112" r:id="rId78" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="A113" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="A114" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="A115" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="A116" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="A117" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="A118" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="A120" r:id="rId85" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="A121" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="A123" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="A124" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="A125" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="A126" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="A127" r:id="rId91" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="D3" r:id="rId92" display="http://sabose.cu/" xr:uid="{47EDC6A2-E374-4384-83BF-1151296A8B80}"/>
+    <hyperlink ref="D21" r:id="rId93" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{8191FBBF-8854-4C0A-8B84-E84F0CC1A943}"/>
+    <hyperlink ref="D24" r:id="rId94" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{BBD40848-FBCD-4DBE-ADBF-830C639AC43C}"/>
+    <hyperlink ref="D23" r:id="rId95" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{E347D519-C1BE-4E2F-9DE2-4F876CAA1896}"/>
+    <hyperlink ref="D22" r:id="rId96" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{099130F4-96CB-41A1-AF6B-E959DE9F4517}"/>
+    <hyperlink ref="D37" r:id="rId97" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTMwMDAmb3JnSWQ9MTQ2NzU0&amp;person_id=22297698&amp;forPersonCustId=3000" xr:uid="{850A56CE-02C6-4335-82D5-BC8FCA19D520}"/>
+    <hyperlink ref="D40" r:id="rId98" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=21687687&amp;forPersonCustId=3000" xr:uid="{2E221ED3-44BB-4C33-B120-4A5DC7FC4D0C}"/>
+    <hyperlink ref="D41" r:id="rId99" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{90032F47-9BAC-4D8F-9DEB-338BF29E04F2}"/>
+    <hyperlink ref="D42" r:id="rId100" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{1D2F84AA-1DE0-4251-9DAE-1EF798CFEFBC}"/>
+    <hyperlink ref="D43" r:id="rId101" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{AD4A5868-800F-42DC-8BEC-9F2A06319281}"/>
+    <hyperlink ref="D83" r:id="rId102" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=6929346&amp;forPersonCustId=47" xr:uid="{1EBA4DAD-A644-4D69-939A-195D56E5D254}"/>
+    <hyperlink ref="D84" r:id="rId103" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36889637&amp;forPersonCustId=1400" xr:uid="{AE6AD973-8B2E-45FA-B623-EA01EBEE0AFD}"/>
+    <hyperlink ref="D85" r:id="rId104" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=22433553&amp;forPersonCustId=1400" xr:uid="{962BF6F0-F8E6-4D8B-B56F-CDB12A596BA0}"/>
+    <hyperlink ref="D91" r:id="rId105" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{7FD4B6CF-752F-4666-818B-8BA80FC216F5}"/>
+    <hyperlink ref="D92" r:id="rId106" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{30966F6F-B77C-4914-AB8D-A15DBD0329F5}"/>
+    <hyperlink ref="D108" r:id="rId107" display="http://puchakraborty.cm/" xr:uid="{FB84B2F6-939B-44E5-95B2-C963662FBD0C}"/>
+    <hyperlink ref="A119" r:id="rId108" xr:uid="{2D237A29-BE80-4D01-9992-C2BEB4FB6FC3}"/>
+    <hyperlink ref="A98" r:id="rId109" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="A97" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="A96" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="A95" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="A94" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="A93" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="A92" r:id="rId115" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="A91" r:id="rId116" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="A90" r:id="rId117" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="A89" r:id="rId118" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="A88" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="A87" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="A86" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="A85" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="A84" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A83" r:id="rId124" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="A82" r:id="rId125" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="A81" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="A80" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="A79" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="A78" r:id="rId129" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="A77" r:id="rId130" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="A76" r:id="rId131" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A75" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="A74" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="A73" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="A72" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="A71" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A70" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId139"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId138"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Global search and torrance onshore
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8FB62F-6F7E-47BD-A5D9-C0CFE31D6F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E626CFB7-6E82-4BC3-889A-4095EAF8A3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4620" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="154">
   <si>
     <t>Customer Name</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>25</v>
       </c>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>26</v>
       </c>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>32</v>
       </c>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>59</v>
       </c>
@@ -2748,65 +2748,23 @@
         <v>4400</v>
       </c>
       <c r="C123" t="s">
-        <v>5</v>
-      </c>
-      <c r="D123" s="11"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>59</v>
+        <v>12</v>
+      </c>
+      <c r="D123" s="5">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>153</v>
       </c>
       <c r="B124" s="1">
-        <v>4400</v>
+        <v>5900</v>
       </c>
       <c r="C124" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B125" s="1">
-        <v>4400</v>
-      </c>
-      <c r="C125" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B126" s="1">
-        <v>4400</v>
-      </c>
-      <c r="C126" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B127" s="1">
-        <v>4400</v>
-      </c>
-      <c r="C127" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>153</v>
-      </c>
-      <c r="B128" s="1">
-        <v>5900</v>
-      </c>
-      <c r="C128" t="s">
         <v>12</v>
       </c>
-      <c r="D128" s="5">
+      <c r="D124" s="5">
         <v>99999</v>
       </c>
     </row>
@@ -2899,59 +2857,55 @@
     <hyperlink ref="A120" r:id="rId85" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
     <hyperlink ref="A121" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
     <hyperlink ref="A123" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="A124" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="A125" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="A126" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="A127" r:id="rId91" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="D3" r:id="rId92" display="http://sabose.cu/" xr:uid="{47EDC6A2-E374-4384-83BF-1151296A8B80}"/>
-    <hyperlink ref="D21" r:id="rId93" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{8191FBBF-8854-4C0A-8B84-E84F0CC1A943}"/>
-    <hyperlink ref="D24" r:id="rId94" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{BBD40848-FBCD-4DBE-ADBF-830C639AC43C}"/>
-    <hyperlink ref="D23" r:id="rId95" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{E347D519-C1BE-4E2F-9DE2-4F876CAA1896}"/>
-    <hyperlink ref="D22" r:id="rId96" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{099130F4-96CB-41A1-AF6B-E959DE9F4517}"/>
-    <hyperlink ref="D37" r:id="rId97" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTMwMDAmb3JnSWQ9MTQ2NzU0&amp;person_id=22297698&amp;forPersonCustId=3000" xr:uid="{850A56CE-02C6-4335-82D5-BC8FCA19D520}"/>
-    <hyperlink ref="D40" r:id="rId98" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=21687687&amp;forPersonCustId=3000" xr:uid="{2E221ED3-44BB-4C33-B120-4A5DC7FC4D0C}"/>
-    <hyperlink ref="D41" r:id="rId99" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{90032F47-9BAC-4D8F-9DEB-338BF29E04F2}"/>
-    <hyperlink ref="D42" r:id="rId100" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{1D2F84AA-1DE0-4251-9DAE-1EF798CFEFBC}"/>
-    <hyperlink ref="D43" r:id="rId101" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{AD4A5868-800F-42DC-8BEC-9F2A06319281}"/>
-    <hyperlink ref="D83" r:id="rId102" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=6929346&amp;forPersonCustId=47" xr:uid="{1EBA4DAD-A644-4D69-939A-195D56E5D254}"/>
-    <hyperlink ref="D84" r:id="rId103" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36889637&amp;forPersonCustId=1400" xr:uid="{AE6AD973-8B2E-45FA-B623-EA01EBEE0AFD}"/>
-    <hyperlink ref="D85" r:id="rId104" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=22433553&amp;forPersonCustId=1400" xr:uid="{962BF6F0-F8E6-4D8B-B56F-CDB12A596BA0}"/>
-    <hyperlink ref="D91" r:id="rId105" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{7FD4B6CF-752F-4666-818B-8BA80FC216F5}"/>
-    <hyperlink ref="D92" r:id="rId106" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{30966F6F-B77C-4914-AB8D-A15DBD0329F5}"/>
-    <hyperlink ref="D108" r:id="rId107" display="http://puchakraborty.cm/" xr:uid="{FB84B2F6-939B-44E5-95B2-C963662FBD0C}"/>
-    <hyperlink ref="A119" r:id="rId108" xr:uid="{2D237A29-BE80-4D01-9992-C2BEB4FB6FC3}"/>
-    <hyperlink ref="A98" r:id="rId109" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="A97" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="A96" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="A95" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="A94" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="A93" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="A92" r:id="rId115" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="A91" r:id="rId116" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="A90" r:id="rId117" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="A89" r:id="rId118" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="A88" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="A87" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="A86" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="A85" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="A84" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="A83" r:id="rId124" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="A82" r:id="rId125" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="A81" r:id="rId126" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="A80" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="A79" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="A78" r:id="rId129" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="A77" r:id="rId130" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="A76" r:id="rId131" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="A75" r:id="rId132" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="A74" r:id="rId133" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="A73" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="A72" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="A71" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="A70" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="D3" r:id="rId88" display="http://sabose.cu/" xr:uid="{47EDC6A2-E374-4384-83BF-1151296A8B80}"/>
+    <hyperlink ref="D21" r:id="rId89" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{8191FBBF-8854-4C0A-8B84-E84F0CC1A943}"/>
+    <hyperlink ref="D24" r:id="rId90" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{BBD40848-FBCD-4DBE-ADBF-830C639AC43C}"/>
+    <hyperlink ref="D23" r:id="rId91" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{E347D519-C1BE-4E2F-9DE2-4F876CAA1896}"/>
+    <hyperlink ref="D22" r:id="rId92" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{099130F4-96CB-41A1-AF6B-E959DE9F4517}"/>
+    <hyperlink ref="D37" r:id="rId93" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTMwMDAmb3JnSWQ9MTQ2NzU0&amp;person_id=22297698&amp;forPersonCustId=3000" xr:uid="{850A56CE-02C6-4335-82D5-BC8FCA19D520}"/>
+    <hyperlink ref="D40" r:id="rId94" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=21687687&amp;forPersonCustId=3000" xr:uid="{2E221ED3-44BB-4C33-B120-4A5DC7FC4D0C}"/>
+    <hyperlink ref="D41" r:id="rId95" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{90032F47-9BAC-4D8F-9DEB-338BF29E04F2}"/>
+    <hyperlink ref="D42" r:id="rId96" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{1D2F84AA-1DE0-4251-9DAE-1EF798CFEFBC}"/>
+    <hyperlink ref="D43" r:id="rId97" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{AD4A5868-800F-42DC-8BEC-9F2A06319281}"/>
+    <hyperlink ref="D83" r:id="rId98" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=6929346&amp;forPersonCustId=47" xr:uid="{1EBA4DAD-A644-4D69-939A-195D56E5D254}"/>
+    <hyperlink ref="D84" r:id="rId99" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36889637&amp;forPersonCustId=1400" xr:uid="{AE6AD973-8B2E-45FA-B623-EA01EBEE0AFD}"/>
+    <hyperlink ref="D85" r:id="rId100" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=22433553&amp;forPersonCustId=1400" xr:uid="{962BF6F0-F8E6-4D8B-B56F-CDB12A596BA0}"/>
+    <hyperlink ref="D91" r:id="rId101" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{7FD4B6CF-752F-4666-818B-8BA80FC216F5}"/>
+    <hyperlink ref="D92" r:id="rId102" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{30966F6F-B77C-4914-AB8D-A15DBD0329F5}"/>
+    <hyperlink ref="D108" r:id="rId103" display="http://puchakraborty.cm/" xr:uid="{FB84B2F6-939B-44E5-95B2-C963662FBD0C}"/>
+    <hyperlink ref="A119" r:id="rId104" xr:uid="{2D237A29-BE80-4D01-9992-C2BEB4FB6FC3}"/>
+    <hyperlink ref="A98" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="A97" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="A96" r:id="rId107" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="A95" r:id="rId108" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="A94" r:id="rId109" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="A93" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="A92" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="A91" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="A90" r:id="rId113" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="A89" r:id="rId114" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="A88" r:id="rId115" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="A87" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="A86" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="A85" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="A84" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A83" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="A82" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="A81" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="A80" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="A79" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="A78" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="A77" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="A76" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A75" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="A74" r:id="rId129" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="A73" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="A72" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="A71" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A70" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId138"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId134"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Adding Change Healthcare to CustomerDB.xlsx
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0401E93C-FFF7-4075-8499-19D5FDBFE33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC7283-FE1C-4C05-9206-A1D7E01B657A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="165">
   <si>
     <t>Customer Name</t>
   </si>
@@ -514,6 +514,12 @@
   </si>
   <si>
     <t>Optum Care Colorado(NWST)</t>
+  </si>
+  <si>
+    <t>Change Healthcare</t>
+  </si>
+  <si>
+    <t>change_Anrios</t>
   </si>
 </sst>
 </file>
@@ -1029,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1312,48 +1318,48 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>15</v>
+        <v>163</v>
       </c>
       <c r="B19" s="10">
-        <v>4700</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="10">
-        <v>99999</v>
+        <v>7100</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="10">
+        <v>4700</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="10">
+        <v>99999</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B21" s="10">
         <v>7500</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="10">
-        <v>3200</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>65</v>
+      <c r="D21" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1364,11 +1370,11 @@
       <c r="B22" s="10">
         <v>3200</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>8</v>
+      <c r="C22" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -1379,26 +1385,26 @@
       <c r="B23" s="10">
         <v>3200</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>67</v>
+      <c r="C23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="10">
-        <v>3100</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>5</v>
+        <v>3200</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" s="1"/>
     </row>
@@ -1409,11 +1415,11 @@
       <c r="B25" s="10">
         <v>3100</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>8</v>
+      <c r="C25" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="1"/>
     </row>
@@ -1424,26 +1430,26 @@
       <c r="B26" s="10">
         <v>3100</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>14</v>
+      <c r="C26" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="10">
-        <v>1700</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>71</v>
+        <v>3100</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E27" s="1"/>
     </row>
@@ -1454,11 +1460,11 @@
       <c r="B28" s="10">
         <v>1700</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>8</v>
+      <c r="C28" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="1"/>
     </row>
@@ -1469,26 +1475,26 @@
       <c r="B29" s="10">
         <v>1700</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>9</v>
+      <c r="C29" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="10">
-        <v>2900</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>5</v>
+        <v>1700</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="E30" s="1"/>
     </row>
@@ -1499,11 +1505,11 @@
       <c r="B31" s="10">
         <v>2900</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>14</v>
+      <c r="C31" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E31" s="1"/>
     </row>
@@ -1514,26 +1520,26 @@
       <c r="B32" s="10">
         <v>2900</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>6</v>
+      <c r="C32" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B33" s="10">
-        <v>1800</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>5</v>
+        <v>2900</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -1544,11 +1550,11 @@
       <c r="B34" s="10">
         <v>1800</v>
       </c>
-      <c r="C34" s="14" t="s">
-        <v>8</v>
+      <c r="C34" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" s="1"/>
     </row>
@@ -1559,11 +1565,11 @@
       <c r="B35" s="10">
         <v>1800</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>14</v>
+      <c r="C35" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E35" s="1"/>
     </row>
@@ -1574,41 +1580,41 @@
       <c r="B36" s="10">
         <v>1800</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>6</v>
+      <c r="C36" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" s="10">
-        <v>4300</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>143</v>
+        <v>1800</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="10">
-        <v>3000</v>
+        <v>4300</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="17" t="s">
-        <v>78</v>
+      <c r="D38" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="E38" s="1"/>
     </row>
@@ -1619,11 +1625,11 @@
       <c r="B39" s="10">
         <v>3000</v>
       </c>
-      <c r="C39" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>144</v>
+      <c r="C39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="E39" s="1"/>
     </row>
@@ -1634,11 +1640,11 @@
       <c r="B40" s="10">
         <v>3000</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>145</v>
+      <c r="C40" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="E40" s="1"/>
     </row>
@@ -1649,11 +1655,11 @@
       <c r="B41" s="10">
         <v>3000</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>14</v>
+      <c r="C41" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E41" s="1"/>
     </row>
@@ -1664,26 +1670,26 @@
       <c r="B42" s="10">
         <v>3000</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>79</v>
+      <c r="C42" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B43" s="10">
-        <v>3500</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>80</v>
+        <v>3000</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="E43" s="1"/>
     </row>
@@ -1694,11 +1700,11 @@
       <c r="B44" s="10">
         <v>3500</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>8</v>
+      <c r="C44" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E44" s="1"/>
     </row>
@@ -1709,35 +1715,35 @@
       <c r="B45" s="10">
         <v>3500</v>
       </c>
-      <c r="C45" s="16" t="s">
-        <v>14</v>
+      <c r="C45" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B46" s="10">
-        <v>200</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="10">
-        <v>99999</v>
+        <v>3500</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B47" s="10">
-        <v>3600</v>
+        <v>200</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>12</v>
@@ -1749,16 +1755,16 @@
     </row>
     <row r="48" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B48" s="10">
-        <v>4600</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>83</v>
+        <v>3600</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="10">
+        <v>99999</v>
       </c>
       <c r="E48" s="1"/>
     </row>
@@ -1769,11 +1775,11 @@
       <c r="B49" s="10">
         <v>4600</v>
       </c>
-      <c r="C49" s="14" t="s">
-        <v>8</v>
+      <c r="C49" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E49" s="1"/>
     </row>
@@ -1784,11 +1790,11 @@
       <c r="B50" s="10">
         <v>4600</v>
       </c>
-      <c r="C50" s="15" t="s">
-        <v>9</v>
+      <c r="C50" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E50" s="1"/>
     </row>
@@ -1799,26 +1805,26 @@
       <c r="B51" s="10">
         <v>4600</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>6</v>
+      <c r="C51" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>147</v>
+        <v>85</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B52" s="10">
-        <v>150</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>5</v>
+        <v>4600</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E52" s="1"/>
     </row>
@@ -1829,11 +1835,11 @@
       <c r="B53" s="10">
         <v>150</v>
       </c>
-      <c r="C53" s="14" t="s">
-        <v>8</v>
+      <c r="C53" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E53" s="1"/>
     </row>
@@ -1844,11 +1850,11 @@
       <c r="B54" s="10">
         <v>150</v>
       </c>
-      <c r="C54" s="15" t="s">
-        <v>9</v>
+      <c r="C54" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E54" s="1"/>
     </row>
@@ -1859,11 +1865,11 @@
       <c r="B55" s="10">
         <v>150</v>
       </c>
-      <c r="C55" s="16" t="s">
-        <v>14</v>
+      <c r="C55" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E55" s="1"/>
     </row>
@@ -1874,26 +1880,26 @@
       <c r="B56" s="10">
         <v>150</v>
       </c>
-      <c r="C56" s="13" t="s">
-        <v>6</v>
+      <c r="C56" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B57" s="10">
-        <v>2700</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="E57" s="1"/>
     </row>
@@ -1904,35 +1910,35 @@
       <c r="B58" s="10">
         <v>2700</v>
       </c>
-      <c r="C58" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>154</v>
+      <c r="C58" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="10">
+        <v>2700</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B59" s="10">
+      <c r="B60" s="10">
         <v>2000</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" s="10">
-        <v>99999</v>
-      </c>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B60" s="10">
-        <v>2100</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>12</v>
@@ -1942,18 +1948,18 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
-        <v>126</v>
+        <v>33</v>
       </c>
       <c r="B61" s="10">
-        <v>5600</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>127</v>
+        <v>2100</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="10">
+        <v>99999</v>
       </c>
       <c r="E61" s="1"/>
     </row>
@@ -1964,41 +1970,41 @@
       <c r="B62" s="10">
         <v>5600</v>
       </c>
-      <c r="C62" s="14" t="s">
-        <v>8</v>
+      <c r="C62" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="B63" s="10">
-        <v>2600</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" s="10">
-        <v>99999</v>
+        <v>5600</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B64" s="10">
-        <v>1100</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>86</v>
+        <v>2600</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="10">
+        <v>99999</v>
       </c>
       <c r="E64" s="1"/>
     </row>
@@ -2009,11 +2015,11 @@
       <c r="B65" s="10">
         <v>1100</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>8</v>
+      <c r="C65" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E65" s="1"/>
     </row>
@@ -2024,11 +2030,11 @@
       <c r="B66" s="10">
         <v>1100</v>
       </c>
-      <c r="C66" s="15" t="s">
-        <v>9</v>
+      <c r="C66" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E66" s="1"/>
     </row>
@@ -2039,35 +2045,35 @@
       <c r="B67" s="10">
         <v>1100</v>
       </c>
-      <c r="C67" s="13" t="s">
-        <v>6</v>
+      <c r="C67" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B68" s="10">
-        <v>3300</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="10">
-        <v>99999</v>
+        <v>1100</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B69" s="10">
-        <v>5100</v>
+        <v>3300</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>12</v>
@@ -2079,10 +2085,10 @@
     </row>
     <row r="70" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B70" s="10">
-        <v>7400</v>
+        <v>5100</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>12</v>
@@ -2092,12 +2098,12 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
-        <v>162</v>
+        <v>38</v>
       </c>
       <c r="B71" s="10">
-        <v>2800</v>
+        <v>7400</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>12</v>
@@ -2109,10 +2115,10 @@
     </row>
     <row r="72" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="B72" s="10">
-        <v>5200</v>
+        <v>2800</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>12</v>
@@ -2124,10 +2130,10 @@
     </row>
     <row r="73" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B73" s="10">
-        <v>4800</v>
+        <v>5200</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>12</v>
@@ -2139,10 +2145,10 @@
     </row>
     <row r="74" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="B74" s="10">
-        <v>5300</v>
+        <v>4800</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>12</v>
@@ -2154,10 +2160,10 @@
     </row>
     <row r="75" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="B75" s="10">
-        <v>4900</v>
+        <v>5300</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>12</v>
@@ -2169,10 +2175,10 @@
     </row>
     <row r="76" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
-        <v>133</v>
+        <v>41</v>
       </c>
       <c r="B76" s="10">
-        <v>6600</v>
+        <v>4900</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>12</v>
@@ -2182,12 +2188,12 @@
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="B77" s="10">
-        <v>4100</v>
+        <v>6600</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>12</v>
@@ -2199,10 +2205,10 @@
     </row>
     <row r="78" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B78" s="10">
-        <v>5000</v>
+        <v>4100</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>12</v>
@@ -2214,10 +2220,10 @@
     </row>
     <row r="79" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B79" s="10">
-        <v>4500</v>
+        <v>5000</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>12</v>
@@ -2229,10 +2235,10 @@
     </row>
     <row r="80" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B80" s="10">
-        <v>3400</v>
+        <v>4500</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>12</v>
@@ -2244,16 +2250,16 @@
     </row>
     <row r="81" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B81" s="10">
-        <v>1200</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>90</v>
+        <v>3400</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" s="10">
+        <v>99999</v>
       </c>
       <c r="E81" s="1"/>
     </row>
@@ -2264,11 +2270,11 @@
       <c r="B82" s="10">
         <v>1200</v>
       </c>
-      <c r="C82" s="12" t="s">
-        <v>5</v>
+      <c r="C82" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E82" s="1"/>
     </row>
@@ -2279,11 +2285,11 @@
       <c r="B83" s="10">
         <v>1200</v>
       </c>
-      <c r="C83" s="14" t="s">
-        <v>8</v>
+      <c r="C83" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E83" s="1"/>
     </row>
@@ -2294,26 +2300,26 @@
       <c r="B84" s="10">
         <v>1200</v>
       </c>
-      <c r="C84" s="15" t="s">
-        <v>9</v>
+      <c r="C84" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B85" s="10">
-        <v>3900</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>5</v>
+        <v>1200</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E85" s="1"/>
     </row>
@@ -2324,11 +2330,11 @@
       <c r="B86" s="10">
         <v>3900</v>
       </c>
-      <c r="C86" s="15" t="s">
-        <v>9</v>
+      <c r="C86" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E86" s="1"/>
     </row>
@@ -2339,11 +2345,11 @@
       <c r="B87" s="10">
         <v>3900</v>
       </c>
-      <c r="C87" s="16" t="s">
-        <v>14</v>
+      <c r="C87" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E87" s="1"/>
     </row>
@@ -2354,26 +2360,26 @@
       <c r="B88" s="10">
         <v>3900</v>
       </c>
-      <c r="C88" s="13" t="s">
-        <v>6</v>
+      <c r="C88" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B89" s="10">
-        <v>3800</v>
-      </c>
-      <c r="C89" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>98</v>
+        <v>3900</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="E89" s="1"/>
     </row>
@@ -2384,26 +2390,26 @@
       <c r="B90" s="10">
         <v>3800</v>
       </c>
-      <c r="C90" s="16" t="s">
-        <v>14</v>
+      <c r="C90" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B91" s="10">
-        <v>1300</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>100</v>
+        <v>3800</v>
+      </c>
+      <c r="C91" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E91" s="1"/>
     </row>
@@ -2414,11 +2420,11 @@
       <c r="B92" s="10">
         <v>1300</v>
       </c>
-      <c r="C92" s="14" t="s">
-        <v>8</v>
+      <c r="C92" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E92" s="1"/>
     </row>
@@ -2429,11 +2435,11 @@
       <c r="B93" s="10">
         <v>1300</v>
       </c>
-      <c r="C93" s="15" t="s">
-        <v>9</v>
+      <c r="C93" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E93" s="1"/>
     </row>
@@ -2444,11 +2450,11 @@
       <c r="B94" s="10">
         <v>1300</v>
       </c>
-      <c r="C94" s="16" t="s">
-        <v>14</v>
+      <c r="C94" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E94" s="1"/>
     </row>
@@ -2459,26 +2465,26 @@
       <c r="B95" s="10">
         <v>1300</v>
       </c>
-      <c r="C95" s="13" t="s">
-        <v>6</v>
+      <c r="C95" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B96" s="10">
-        <v>2500</v>
-      </c>
-      <c r="C96" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>105</v>
+        <v>1300</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -2489,11 +2495,11 @@
       <c r="B97" s="10">
         <v>2500</v>
       </c>
-      <c r="C97" s="12" t="s">
-        <v>5</v>
+      <c r="C97" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E97" s="1"/>
     </row>
@@ -2504,26 +2510,26 @@
       <c r="B98" s="10">
         <v>2500</v>
       </c>
-      <c r="C98" s="14" t="s">
-        <v>8</v>
+      <c r="C98" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B99" s="10">
-        <v>6000</v>
-      </c>
-      <c r="C99" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>108</v>
+        <v>2500</v>
+      </c>
+      <c r="C99" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="E99" s="1"/>
     </row>
@@ -2534,11 +2540,11 @@
       <c r="B100" s="10">
         <v>6000</v>
       </c>
-      <c r="C100" s="14" t="s">
-        <v>8</v>
+      <c r="C100" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E100" s="1"/>
     </row>
@@ -2549,26 +2555,26 @@
       <c r="B101" s="10">
         <v>6000</v>
       </c>
-      <c r="C101" s="16" t="s">
+      <c r="C101" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B102" s="10">
+        <v>6000</v>
+      </c>
+      <c r="C102" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D102" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="E101" s="1"/>
-    </row>
-    <row r="102" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B102" s="10">
-        <v>5400</v>
-      </c>
-      <c r="C102" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="E102" s="1"/>
     </row>
@@ -2579,11 +2585,11 @@
       <c r="B103" s="10">
         <v>5400</v>
       </c>
-      <c r="C103" s="12" t="s">
-        <v>5</v>
+      <c r="C103" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E103" s="1"/>
     </row>
@@ -2594,26 +2600,26 @@
       <c r="B104" s="10">
         <v>5400</v>
       </c>
-      <c r="C104" s="16" t="s">
+      <c r="C104" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B105" s="10">
+        <v>5400</v>
+      </c>
+      <c r="C105" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="E104" s="1"/>
-    </row>
-    <row r="105" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B105" s="10">
-        <v>1000</v>
-      </c>
-      <c r="C105" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="E105" s="1"/>
     </row>
@@ -2624,11 +2630,11 @@
       <c r="B106" s="10">
         <v>1000</v>
       </c>
-      <c r="C106" s="16" t="s">
-        <v>14</v>
+      <c r="C106" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="E106" s="1"/>
     </row>
@@ -2639,26 +2645,26 @@
       <c r="B107" s="10">
         <v>1000</v>
       </c>
-      <c r="C107" s="13" t="s">
-        <v>6</v>
+      <c r="C107" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B108" s="10">
-        <v>1900</v>
-      </c>
-      <c r="C108" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>113</v>
+        <v>1000</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="E108" s="1"/>
     </row>
@@ -2669,11 +2675,11 @@
       <c r="B109" s="10">
         <v>1900</v>
       </c>
-      <c r="C109" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>114</v>
+      <c r="C109" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="E109" s="1"/>
     </row>
@@ -2684,11 +2690,11 @@
       <c r="B110" s="10">
         <v>1900</v>
       </c>
-      <c r="C110" s="15" t="s">
-        <v>9</v>
+      <c r="C110" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E110" s="1"/>
     </row>
@@ -2699,11 +2705,11 @@
       <c r="B111" s="10">
         <v>1900</v>
       </c>
-      <c r="C111" s="16" t="s">
-        <v>14</v>
+      <c r="C111" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E111" s="1"/>
     </row>
@@ -2714,41 +2720,41 @@
       <c r="B112" s="10">
         <v>1900</v>
       </c>
-      <c r="C112" s="13" t="s">
+      <c r="C112" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E112" s="1"/>
+    </row>
+    <row r="113" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B113" s="10">
+        <v>1900</v>
+      </c>
+      <c r="C113" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D113" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E112" s="1"/>
-    </row>
-    <row r="113" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="9" t="s">
+      <c r="E113" s="1"/>
+    </row>
+    <row r="114" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B113" s="10">
+      <c r="B114" s="10">
         <v>7000</v>
       </c>
-      <c r="C113" s="11" t="s">
+      <c r="C114" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D113" s="10">
+      <c r="D114" s="10">
         <v>99999</v>
-      </c>
-      <c r="E113" s="1"/>
-    </row>
-    <row r="114" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B114" s="10">
-        <v>4000</v>
-      </c>
-      <c r="C114" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="E114" s="1"/>
     </row>
@@ -2759,11 +2765,11 @@
       <c r="B115" s="10">
         <v>4000</v>
       </c>
-      <c r="C115" s="15" t="s">
-        <v>9</v>
+      <c r="C115" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E115" s="1"/>
     </row>
@@ -2774,26 +2780,26 @@
       <c r="B116" s="10">
         <v>4000</v>
       </c>
-      <c r="C116" s="16" t="s">
-        <v>14</v>
+      <c r="C116" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B117" s="10">
-        <v>6500</v>
-      </c>
-      <c r="C117" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>105</v>
+        <v>4000</v>
+      </c>
+      <c r="C117" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="E117" s="1"/>
     </row>
@@ -2804,11 +2810,11 @@
       <c r="B118" s="10">
         <v>6500</v>
       </c>
-      <c r="C118" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D118" s="7" t="s">
-        <v>121</v>
+      <c r="C118" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="E118" s="1"/>
     </row>
@@ -2819,11 +2825,11 @@
       <c r="B119" s="10">
         <v>6500</v>
       </c>
-      <c r="C119" s="14" t="s">
-        <v>8</v>
+      <c r="C119" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E119" s="1"/>
     </row>
@@ -2834,11 +2840,11 @@
       <c r="B120" s="10">
         <v>6500</v>
       </c>
-      <c r="C120" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>123</v>
+      <c r="C120" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="E120" s="1"/>
     </row>
@@ -2849,11 +2855,11 @@
       <c r="B121" s="10">
         <v>6500</v>
       </c>
-      <c r="C121" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>124</v>
+      <c r="C121" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2864,34 +2870,35 @@
       <c r="B122" s="10">
         <v>6500</v>
       </c>
-      <c r="C122" s="13" t="s">
-        <v>6</v>
+      <c r="C122" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="9" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="B123" s="10">
-        <v>5800</v>
-      </c>
-      <c r="C123" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D123" s="10">
-        <v>99999</v>
-      </c>
+        <v>6500</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="9" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="B124" s="10">
-        <v>4400</v>
+        <v>5800</v>
       </c>
       <c r="C124" s="11" t="s">
         <v>12</v>
@@ -2902,10 +2909,10 @@
     </row>
     <row r="125" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="9" t="s">
-        <v>131</v>
+        <v>57</v>
       </c>
       <c r="B125" s="10">
-        <v>5900</v>
+        <v>4400</v>
       </c>
       <c r="C125" s="11" t="s">
         <v>12</v>
@@ -2914,19 +2921,33 @@
         <v>99999</v>
       </c>
     </row>
+    <row r="126" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B126" s="10">
+        <v>5900</v>
+      </c>
+      <c r="C126" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D126" s="10">
+        <v>99999</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D23" r:id="rId1" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{76D85841-0E92-4011-A17D-A4C4F39B78A0}"/>
-    <hyperlink ref="D24" r:id="rId2" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{C9A79CA9-B167-443A-AB21-1EA20451173E}"/>
-    <hyperlink ref="D25" r:id="rId3" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{6D2A01E7-99B9-4DCA-8F10-0193BA4220F1}"/>
-    <hyperlink ref="D26" r:id="rId4" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{53D741C5-74C7-42B4-8631-E0FC11F4CAA7}"/>
-    <hyperlink ref="D43" r:id="rId5" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{22C1094A-0EAE-42D9-B543-021DD6A2C36F}"/>
-    <hyperlink ref="D44" r:id="rId6" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{7E462E08-4B0C-476D-AA36-E11FA80272FA}"/>
-    <hyperlink ref="D45" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{13B4A8AE-B629-42F9-B867-9E81A7263C7A}"/>
-    <hyperlink ref="D89" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{C28604FE-26D1-453D-8E55-BF4C270F28C4}"/>
-    <hyperlink ref="D90" r:id="rId9" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{E9917C5C-D5F0-4AD9-A2ED-472C92E6011C}"/>
-    <hyperlink ref="D108" r:id="rId10" display="http://puchakraborty.cm/" xr:uid="{02AFB277-C913-480D-BB5B-879E6BB17D14}"/>
-    <hyperlink ref="D20" r:id="rId11" xr:uid="{FCE7A3BF-4446-4E9F-83A0-11A360F0A079}"/>
+    <hyperlink ref="D24" r:id="rId1" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{76D85841-0E92-4011-A17D-A4C4F39B78A0}"/>
+    <hyperlink ref="D25" r:id="rId2" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{C9A79CA9-B167-443A-AB21-1EA20451173E}"/>
+    <hyperlink ref="D26" r:id="rId3" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{6D2A01E7-99B9-4DCA-8F10-0193BA4220F1}"/>
+    <hyperlink ref="D27" r:id="rId4" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{53D741C5-74C7-42B4-8631-E0FC11F4CAA7}"/>
+    <hyperlink ref="D44" r:id="rId5" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{22C1094A-0EAE-42D9-B543-021DD6A2C36F}"/>
+    <hyperlink ref="D45" r:id="rId6" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{7E462E08-4B0C-476D-AA36-E11FA80272FA}"/>
+    <hyperlink ref="D46" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{13B4A8AE-B629-42F9-B867-9E81A7263C7A}"/>
+    <hyperlink ref="D90" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{C28604FE-26D1-453D-8E55-BF4C270F28C4}"/>
+    <hyperlink ref="D91" r:id="rId9" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{E9917C5C-D5F0-4AD9-A2ED-472C92E6011C}"/>
+    <hyperlink ref="D109" r:id="rId10" display="http://puchakraborty.cm/" xr:uid="{02AFB277-C913-480D-BB5B-879E6BB17D14}"/>
+    <hyperlink ref="D21" r:id="rId11" xr:uid="{FCE7A3BF-4446-4E9F-83A0-11A360F0A079}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>

</xml_diff>

<commit_message>
Adding OCKS and OCID
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC7283-FE1C-4C05-9206-A1D7E01B657A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAE3B3D-55A5-4466-A6E8-5FA640CCE036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="167">
   <si>
     <t>Customer Name</t>
   </si>
@@ -520,6 +520,12 @@
   </si>
   <si>
     <t>change_Anrios</t>
+  </si>
+  <si>
+    <t>Optum Care Network - Idaho</t>
+  </si>
+  <si>
+    <t>Optum Kansas City</t>
   </si>
 </sst>
 </file>
@@ -636,7 +642,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -659,12 +665,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -719,6 +736,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1035,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1068,7 @@
     <col min="4" max="4" width="34.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1138,7 +1158,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1183,7 +1203,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
@@ -1258,7 +1278,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
@@ -1273,7 +1293,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
@@ -1393,7 +1413,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>16</v>
       </c>
@@ -1438,7 +1458,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>17</v>
       </c>
@@ -1483,7 +1503,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>18</v>
       </c>
@@ -1513,7 +1533,7 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>19</v>
       </c>
@@ -1573,7 +1593,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>23</v>
       </c>
@@ -1648,7 +1668,7 @@
       </c>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>25</v>
       </c>
@@ -1663,7 +1683,7 @@
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>25</v>
       </c>
@@ -1723,7 +1743,7 @@
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>26</v>
       </c>
@@ -1798,7 +1818,7 @@
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>29</v>
       </c>
@@ -1858,7 +1878,7 @@
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>30</v>
       </c>
@@ -1873,7 +1893,7 @@
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>30</v>
       </c>
@@ -2130,10 +2150,10 @@
     </row>
     <row r="73" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B73" s="10">
-        <v>5200</v>
+        <v>165</v>
+      </c>
+      <c r="B73" s="19">
+        <v>1550</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>12</v>
@@ -2141,14 +2161,13 @@
       <c r="D73" s="10">
         <v>99999</v>
       </c>
-      <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="B74" s="10">
-        <v>4800</v>
+        <v>6600</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>12</v>
@@ -2160,10 +2179,10 @@
     </row>
     <row r="75" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
-        <v>125</v>
+        <v>39</v>
       </c>
       <c r="B75" s="10">
-        <v>5300</v>
+        <v>5200</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>12</v>
@@ -2175,10 +2194,10 @@
     </row>
     <row r="76" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B76" s="10">
-        <v>4900</v>
+        <v>4800</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>12</v>
@@ -2190,10 +2209,10 @@
     </row>
     <row r="77" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B77" s="10">
-        <v>6600</v>
+        <v>5300</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>12</v>
@@ -2203,12 +2222,12 @@
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B78" s="10">
-        <v>4100</v>
+        <v>4900</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>12</v>
@@ -2220,10 +2239,10 @@
     </row>
     <row r="79" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B79" s="10">
-        <v>5000</v>
+        <v>4100</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>12</v>
@@ -2235,10 +2254,10 @@
     </row>
     <row r="80" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B80" s="10">
-        <v>4500</v>
+        <v>5000</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>12</v>
@@ -2250,10 +2269,10 @@
     </row>
     <row r="81" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B81" s="10">
-        <v>3400</v>
+        <v>166</v>
+      </c>
+      <c r="B81" s="19">
+        <v>1650</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>12</v>
@@ -2261,35 +2280,34 @@
       <c r="D81" s="10">
         <v>99999</v>
       </c>
-      <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B82" s="10">
-        <v>1200</v>
-      </c>
-      <c r="C82" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>90</v>
+        <v>4500</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D82" s="10">
+        <v>99999</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B83" s="10">
-        <v>1200</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>91</v>
+        <v>3400</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" s="10">
+        <v>99999</v>
       </c>
       <c r="E83" s="1"/>
     </row>
@@ -2300,11 +2318,11 @@
       <c r="B84" s="10">
         <v>1200</v>
       </c>
-      <c r="C84" s="14" t="s">
-        <v>8</v>
+      <c r="C84" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E84" s="1"/>
     </row>
@@ -2315,41 +2333,41 @@
       <c r="B85" s="10">
         <v>1200</v>
       </c>
-      <c r="C85" s="15" t="s">
-        <v>9</v>
+      <c r="C85" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B86" s="10">
-        <v>3900</v>
-      </c>
-      <c r="C86" s="12" t="s">
-        <v>5</v>
+        <v>1200</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B87" s="10">
-        <v>3900</v>
+        <v>1200</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E87" s="1"/>
     </row>
@@ -2360,11 +2378,11 @@
       <c r="B88" s="10">
         <v>3900</v>
       </c>
-      <c r="C88" s="16" t="s">
-        <v>14</v>
+      <c r="C88" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -2375,71 +2393,71 @@
       <c r="B89" s="10">
         <v>3900</v>
       </c>
-      <c r="C89" s="13" t="s">
-        <v>6</v>
+      <c r="C89" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B90" s="10">
-        <v>3800</v>
-      </c>
-      <c r="C90" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>98</v>
+        <v>3900</v>
+      </c>
+      <c r="C90" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B91" s="10">
-        <v>3800</v>
-      </c>
-      <c r="C91" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>99</v>
+        <v>3900</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B92" s="10">
-        <v>1300</v>
+        <v>3800</v>
       </c>
       <c r="C92" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>100</v>
+      <c r="D92" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B93" s="10">
-        <v>1300</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>101</v>
+        <v>3800</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E93" s="1"/>
     </row>
@@ -2450,11 +2468,11 @@
       <c r="B94" s="10">
         <v>1300</v>
       </c>
-      <c r="C94" s="15" t="s">
-        <v>9</v>
+      <c r="C94" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E94" s="1"/>
     </row>
@@ -2465,11 +2483,11 @@
       <c r="B95" s="10">
         <v>1300</v>
       </c>
-      <c r="C95" s="16" t="s">
-        <v>14</v>
+      <c r="C95" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E95" s="1"/>
     </row>
@@ -2480,41 +2498,41 @@
       <c r="B96" s="10">
         <v>1300</v>
       </c>
-      <c r="C96" s="13" t="s">
-        <v>6</v>
+      <c r="C96" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B97" s="10">
-        <v>2500</v>
-      </c>
-      <c r="C97" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>105</v>
+        <v>1300</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B98" s="10">
-        <v>2500</v>
-      </c>
-      <c r="C98" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>106</v>
+        <v>1300</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="E98" s="1"/>
     </row>
@@ -2525,41 +2543,41 @@
       <c r="B99" s="10">
         <v>2500</v>
       </c>
-      <c r="C99" s="14" t="s">
-        <v>8</v>
+      <c r="C99" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B100" s="10">
-        <v>6000</v>
+        <v>2500</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>108</v>
+      <c r="D100" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B101" s="10">
-        <v>6000</v>
+        <v>2500</v>
       </c>
       <c r="C101" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>109</v>
+      <c r="D101" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="E101" s="1"/>
     </row>
@@ -2570,41 +2588,41 @@
       <c r="B102" s="10">
         <v>6000</v>
       </c>
-      <c r="C102" s="16" t="s">
-        <v>14</v>
+      <c r="C102" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="B103" s="10">
-        <v>5400</v>
+        <v>6000</v>
       </c>
       <c r="C103" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="B104" s="10">
-        <v>5400</v>
-      </c>
-      <c r="C104" s="12" t="s">
-        <v>5</v>
+        <v>6000</v>
+      </c>
+      <c r="C104" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="E104" s="1"/>
     </row>
@@ -2615,41 +2633,41 @@
       <c r="B105" s="10">
         <v>5400</v>
       </c>
-      <c r="C105" s="16" t="s">
-        <v>14</v>
+      <c r="C105" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E105" s="1"/>
     </row>
-    <row r="106" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="B106" s="10">
-        <v>1000</v>
+        <v>5400</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="B107" s="10">
-        <v>1000</v>
+        <v>5400</v>
       </c>
       <c r="C107" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="E107" s="1"/>
     </row>
@@ -2660,41 +2678,41 @@
       <c r="B108" s="10">
         <v>1000</v>
       </c>
-      <c r="C108" s="13" t="s">
-        <v>6</v>
+      <c r="C108" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B109" s="10">
-        <v>1900</v>
-      </c>
-      <c r="C109" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>113</v>
+        <v>1000</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B110" s="10">
-        <v>1900</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>8</v>
+        <v>1000</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E110" s="1"/>
     </row>
@@ -2705,11 +2723,11 @@
       <c r="B111" s="10">
         <v>1900</v>
       </c>
-      <c r="C111" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>115</v>
+      <c r="C111" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="E111" s="1"/>
     </row>
@@ -2720,11 +2738,11 @@
       <c r="B112" s="10">
         <v>1900</v>
       </c>
-      <c r="C112" s="16" t="s">
-        <v>14</v>
+      <c r="C112" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2735,56 +2753,56 @@
       <c r="B113" s="10">
         <v>1900</v>
       </c>
-      <c r="C113" s="13" t="s">
-        <v>6</v>
+      <c r="C113" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="9" t="s">
-        <v>136</v>
+        <v>54</v>
       </c>
       <c r="B114" s="10">
-        <v>7000</v>
-      </c>
-      <c r="C114" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D114" s="10">
-        <v>99999</v>
+        <v>1900</v>
+      </c>
+      <c r="C114" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B115" s="10">
-        <v>4000</v>
-      </c>
-      <c r="C115" s="12" t="s">
-        <v>5</v>
+        <v>1900</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E115" s="1"/>
     </row>
-    <row r="116" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="9" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="B116" s="10">
-        <v>4000</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>119</v>
+        <v>7000</v>
+      </c>
+      <c r="C116" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" s="10">
+        <v>99999</v>
       </c>
       <c r="E116" s="1"/>
     </row>
@@ -2795,41 +2813,41 @@
       <c r="B117" s="10">
         <v>4000</v>
       </c>
-      <c r="C117" s="16" t="s">
-        <v>14</v>
+      <c r="C117" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B118" s="10">
-        <v>6500</v>
-      </c>
-      <c r="C118" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D118" s="4" t="s">
-        <v>105</v>
+        <v>4000</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B119" s="10">
-        <v>6500</v>
-      </c>
-      <c r="C119" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D119" s="7" t="s">
-        <v>121</v>
+        <v>4000</v>
+      </c>
+      <c r="C119" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="E119" s="1"/>
     </row>
@@ -2840,11 +2858,11 @@
       <c r="B120" s="10">
         <v>6500</v>
       </c>
-      <c r="C120" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>122</v>
+      <c r="C120" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="E120" s="1"/>
     </row>
@@ -2855,11 +2873,11 @@
       <c r="B121" s="10">
         <v>6500</v>
       </c>
-      <c r="C121" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>123</v>
+      <c r="C121" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2870,11 +2888,11 @@
       <c r="B122" s="10">
         <v>6500</v>
       </c>
-      <c r="C122" s="16" t="s">
-        <v>14</v>
+      <c r="C122" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E122" s="1"/>
     </row>
@@ -2885,53 +2903,83 @@
       <c r="B123" s="10">
         <v>6500</v>
       </c>
-      <c r="C123" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>159</v>
+      <c r="C123" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="9" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="B124" s="10">
-        <v>5800</v>
-      </c>
-      <c r="C124" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D124" s="10">
-        <v>99999</v>
-      </c>
+        <v>6500</v>
+      </c>
+      <c r="C124" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D124" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B125" s="10">
-        <v>4400</v>
-      </c>
-      <c r="C125" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D125" s="10">
-        <v>99999</v>
-      </c>
+        <v>6500</v>
+      </c>
+      <c r="C125" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B126" s="10">
-        <v>5900</v>
+        <v>5800</v>
       </c>
       <c r="C126" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D126" s="10">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B127" s="10">
+        <v>4400</v>
+      </c>
+      <c r="C127" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D127" s="10">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B128" s="10">
+        <v>5900</v>
+      </c>
+      <c r="C128" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D128" s="10">
         <v>99999</v>
       </c>
     </row>
@@ -2944,13 +2992,15 @@
     <hyperlink ref="D44" r:id="rId5" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{22C1094A-0EAE-42D9-B543-021DD6A2C36F}"/>
     <hyperlink ref="D45" r:id="rId6" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{7E462E08-4B0C-476D-AA36-E11FA80272FA}"/>
     <hyperlink ref="D46" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{13B4A8AE-B629-42F9-B867-9E81A7263C7A}"/>
-    <hyperlink ref="D90" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{C28604FE-26D1-453D-8E55-BF4C270F28C4}"/>
-    <hyperlink ref="D91" r:id="rId9" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{E9917C5C-D5F0-4AD9-A2ED-472C92E6011C}"/>
-    <hyperlink ref="D109" r:id="rId10" display="http://puchakraborty.cm/" xr:uid="{02AFB277-C913-480D-BB5B-879E6BB17D14}"/>
+    <hyperlink ref="D92" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{C28604FE-26D1-453D-8E55-BF4C270F28C4}"/>
+    <hyperlink ref="D93" r:id="rId9" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{E9917C5C-D5F0-4AD9-A2ED-472C92E6011C}"/>
+    <hyperlink ref="D111" r:id="rId10" display="http://puchakraborty.cm/" xr:uid="{02AFB277-C913-480D-BB5B-879E6BB17D14}"/>
     <hyperlink ref="D21" r:id="rId11" xr:uid="{FCE7A3BF-4446-4E9F-83A0-11A360F0A079}"/>
+    <hyperlink ref="A73" r:id="rId12" tooltip="Optum Care Network - Idaho" display="javascript:void(0);" xr:uid="{90E131F6-422B-407C-B173-D7B05E9A01F6}"/>
+    <hyperlink ref="A81" r:id="rId13" tooltip="Optum Kansas City" display="javascript:void(0);" xr:uid="{ED7C1925-38C1-4B1C-BD55-4AC2E2B634E2}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Dignity office admin removed
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D11CEFB-5901-4EFD-8626-97A1DC811D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E117531C-9498-4A26-8CF5-0F2459C5EF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-4620" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="166">
   <si>
     <t>Customer Name</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>dhmf_abajwa</t>
-  </si>
-  <si>
-    <t>dignity.familypractice</t>
   </si>
   <si>
     <t>epic_agonzales</t>
@@ -1055,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1082,7 @@
     </row>
     <row r="2" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="10">
         <v>99999</v>
@@ -1109,7 +1106,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -1124,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -1139,7 +1136,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -1154,7 +1151,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -1169,7 +1166,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -1184,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -1235,7 +1232,7 @@
     </row>
     <row r="12" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12" s="10">
         <v>6800</v>
@@ -1325,7 +1322,7 @@
     </row>
     <row r="18" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B18" s="10">
         <v>6700</v>
@@ -1340,7 +1337,7 @@
     </row>
     <row r="19" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" s="10">
         <v>7100</v>
@@ -1349,7 +1346,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -1370,7 +1367,7 @@
     </row>
     <row r="21" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B21" s="10">
         <v>7500</v>
@@ -1379,7 +1376,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1458,17 +1455,17 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B27" s="10">
-        <v>3100</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="5" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>70</v>
       </c>
       <c r="E27" s="1"/>
@@ -1480,86 +1477,86 @@
       <c r="B28" s="10">
         <v>1700</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>5</v>
+      <c r="C28" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="10">
         <v>1700</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>8</v>
+      <c r="C29" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>72</v>
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B30" s="10">
-        <v>1700</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>9</v>
+        <v>2900</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="10">
         <v>2900</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>5</v>
+      <c r="C31" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="10">
         <v>2900</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>14</v>
+      <c r="C32" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B33" s="10">
-        <v>2900</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>6</v>
+        <v>1800</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -1570,38 +1567,38 @@
       <c r="B34" s="10">
         <v>1800</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>5</v>
+      <c r="C34" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="10">
         <v>1800</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>8</v>
+      <c r="C35" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>75</v>
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B36" s="10">
         <v>1800</v>
       </c>
-      <c r="C36" s="16" t="s">
-        <v>14</v>
+      <c r="C36" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>76</v>
@@ -1610,31 +1607,31 @@
     </row>
     <row r="37" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B37" s="10">
-        <v>1800</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>77</v>
+        <v>4300</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B38" s="10">
-        <v>4300</v>
+        <v>3000</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>142</v>
+      <c r="D38" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="E38" s="1"/>
     </row>
@@ -1645,25 +1642,25 @@
       <c r="B39" s="10">
         <v>3000</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>78</v>
+      <c r="C39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B40" s="10">
         <v>3000</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="3" t="s">
+      <c r="C40" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>143</v>
       </c>
       <c r="E40" s="1"/>
@@ -1675,40 +1672,40 @@
       <c r="B41" s="10">
         <v>3000</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>9</v>
+      <c r="C41" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>144</v>
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B42" s="10">
         <v>3000</v>
       </c>
-      <c r="C42" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>145</v>
+      <c r="C42" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B43" s="10">
-        <v>3000</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="17" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E43" s="1"/>
@@ -1720,50 +1717,50 @@
       <c r="B44" s="10">
         <v>3500</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>5</v>
+      <c r="C44" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>80</v>
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B45" s="10">
         <v>3500</v>
       </c>
-      <c r="C45" s="14" t="s">
-        <v>8</v>
+      <c r="C45" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>81</v>
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B46" s="10">
-        <v>3500</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>82</v>
+        <v>200</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="10">
+        <v>99999</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B47" s="10">
-        <v>200</v>
+        <v>3600</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>12</v>
@@ -1775,16 +1772,16 @@
     </row>
     <row r="48" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B48" s="10">
-        <v>3600</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="10">
-        <v>99999</v>
+        <v>4600</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="E48" s="1"/>
     </row>
@@ -1795,53 +1792,53 @@
       <c r="B49" s="10">
         <v>4600</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>5</v>
+      <c r="C49" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B50" s="10">
         <v>4600</v>
       </c>
-      <c r="C50" s="14" t="s">
-        <v>8</v>
+      <c r="C50" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B51" s="10">
         <v>4600</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>9</v>
+      <c r="C51" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B52" s="10">
-        <v>4600</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>6</v>
+        <v>150</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>146</v>
@@ -1855,23 +1852,23 @@
       <c r="B53" s="10">
         <v>150</v>
       </c>
-      <c r="C53" s="12" t="s">
-        <v>5</v>
+      <c r="C53" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B54" s="10">
         <v>150</v>
       </c>
-      <c r="C54" s="14" t="s">
-        <v>8</v>
+      <c r="C54" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>148</v>
@@ -1885,23 +1882,23 @@
       <c r="B55" s="10">
         <v>150</v>
       </c>
-      <c r="C55" s="15" t="s">
-        <v>9</v>
+      <c r="C55" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>149</v>
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B56" s="10">
         <v>150</v>
       </c>
-      <c r="C56" s="16" t="s">
-        <v>14</v>
+      <c r="C56" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>150</v>
@@ -1910,55 +1907,55 @@
     </row>
     <row r="57" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B57" s="10">
-        <v>150</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="3" t="s">
+        <v>2700</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>151</v>
       </c>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B58" s="10">
         <v>2700</v>
       </c>
-      <c r="C58" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="6" t="s">
+      <c r="C58" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>152</v>
       </c>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B59" s="10">
-        <v>2700</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>153</v>
+        <v>2000</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="10">
+        <v>99999</v>
       </c>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B60" s="10">
-        <v>2000</v>
+        <v>2100</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>12</v>
@@ -1968,63 +1965,63 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="B61" s="10">
-        <v>2100</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="10">
-        <v>99999</v>
+        <v>5600</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B62" s="10">
         <v>5600</v>
       </c>
-      <c r="C62" s="12" t="s">
-        <v>5</v>
+      <c r="C62" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="B63" s="10">
-        <v>5600</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>166</v>
+        <v>2600</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="10">
+        <v>99999</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B64" s="10">
-        <v>2600</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64" s="10">
-        <v>99999</v>
+        <v>1100</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="E64" s="1"/>
     </row>
@@ -2035,38 +2032,38 @@
       <c r="B65" s="10">
         <v>1100</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>5</v>
+      <c r="C65" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B66" s="10">
         <v>1100</v>
       </c>
-      <c r="C66" s="14" t="s">
-        <v>8</v>
+      <c r="C66" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B67" s="10">
         <v>1100</v>
       </c>
-      <c r="C67" s="15" t="s">
-        <v>9</v>
+      <c r="C67" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>88</v>
@@ -2075,25 +2072,25 @@
     </row>
     <row r="68" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B68" s="10">
-        <v>1100</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>89</v>
+        <v>3300</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="10">
+        <v>99999</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B69" s="10">
-        <v>3300</v>
+        <v>5100</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>12</v>
@@ -2105,10 +2102,10 @@
     </row>
     <row r="70" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B70" s="10">
-        <v>5100</v>
+        <v>7400</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>12</v>
@@ -2118,12 +2115,12 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="B71" s="10">
-        <v>7400</v>
+        <v>2800</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>12</v>
@@ -2135,10 +2132,10 @@
     </row>
     <row r="72" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="B72" s="10">
-        <v>2800</v>
+        <v>163</v>
+      </c>
+      <c r="B72" s="19">
+        <v>1550</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>12</v>
@@ -2146,14 +2143,13 @@
       <c r="D72" s="10">
         <v>99999</v>
       </c>
-      <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B73" s="19">
-        <v>1550</v>
+        <v>131</v>
+      </c>
+      <c r="B73" s="10">
+        <v>6600</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>12</v>
@@ -2161,13 +2157,14 @@
       <c r="D73" s="10">
         <v>99999</v>
       </c>
+      <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
-        <v>132</v>
+        <v>39</v>
       </c>
       <c r="B74" s="10">
-        <v>6600</v>
+        <v>5200</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>12</v>
@@ -2179,10 +2176,10 @@
     </row>
     <row r="75" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B75" s="10">
-        <v>5200</v>
+        <v>4800</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>12</v>
@@ -2194,10 +2191,10 @@
     </row>
     <row r="76" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="B76" s="10">
-        <v>4800</v>
+        <v>5300</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>12</v>
@@ -2209,10 +2206,10 @@
     </row>
     <row r="77" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="B77" s="10">
-        <v>5300</v>
+        <v>4900</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>12</v>
@@ -2224,10 +2221,10 @@
     </row>
     <row r="78" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B78" s="10">
-        <v>4900</v>
+        <v>4100</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>12</v>
@@ -2237,12 +2234,12 @@
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B79" s="10">
-        <v>4100</v>
+        <v>5000</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>12</v>
@@ -2254,10 +2251,10 @@
     </row>
     <row r="80" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B80" s="10">
-        <v>5000</v>
+        <v>164</v>
+      </c>
+      <c r="B80" s="19">
+        <v>1650</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>12</v>
@@ -2265,14 +2262,13 @@
       <c r="D80" s="10">
         <v>99999</v>
       </c>
-      <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B81" s="19">
-        <v>1650</v>
+        <v>44</v>
+      </c>
+      <c r="B81" s="10">
+        <v>4500</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>12</v>
@@ -2280,13 +2276,14 @@
       <c r="D81" s="10">
         <v>99999</v>
       </c>
+      <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B82" s="10">
-        <v>4500</v>
+        <v>3400</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>12</v>
@@ -2298,16 +2295,16 @@
     </row>
     <row r="83" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B83" s="10">
-        <v>3400</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D83" s="10">
-        <v>99999</v>
+        <v>1200</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="E83" s="1"/>
     </row>
@@ -2318,8 +2315,8 @@
       <c r="B84" s="10">
         <v>1200</v>
       </c>
-      <c r="C84" s="18" t="s">
-        <v>47</v>
+      <c r="C84" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>90</v>
@@ -2333,53 +2330,53 @@
       <c r="B85" s="10">
         <v>1200</v>
       </c>
-      <c r="C85" s="12" t="s">
-        <v>5</v>
+      <c r="C85" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B86" s="10">
         <v>1200</v>
       </c>
-      <c r="C86" s="14" t="s">
-        <v>8</v>
+      <c r="C86" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B87" s="10">
-        <v>1200</v>
-      </c>
-      <c r="C87" s="15" t="s">
-        <v>9</v>
+        <v>3900</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B88" s="10">
         <v>3900</v>
       </c>
-      <c r="C88" s="12" t="s">
-        <v>5</v>
+      <c r="C88" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>94</v>
@@ -2393,23 +2390,23 @@
       <c r="B89" s="10">
         <v>3900</v>
       </c>
-      <c r="C89" s="15" t="s">
-        <v>9</v>
+      <c r="C89" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B90" s="10">
         <v>3900</v>
       </c>
-      <c r="C90" s="16" t="s">
-        <v>14</v>
+      <c r="C90" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>96</v>
@@ -2418,45 +2415,45 @@
     </row>
     <row r="91" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B91" s="10">
-        <v>3900</v>
-      </c>
-      <c r="C91" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="3" t="s">
+        <v>3800</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>97</v>
       </c>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B92" s="10">
         <v>3800</v>
       </c>
-      <c r="C92" s="12" t="s">
-        <v>5</v>
+      <c r="C92" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>98</v>
       </c>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B93" s="10">
-        <v>3800</v>
-      </c>
-      <c r="C93" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D93" s="5" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E93" s="1"/>
@@ -2468,23 +2465,23 @@
       <c r="B94" s="10">
         <v>1300</v>
       </c>
-      <c r="C94" s="12" t="s">
-        <v>5</v>
+      <c r="C94" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B95" s="10">
         <v>1300</v>
       </c>
-      <c r="C95" s="14" t="s">
-        <v>8</v>
+      <c r="C95" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>101</v>
@@ -2498,23 +2495,23 @@
       <c r="B96" s="10">
         <v>1300</v>
       </c>
-      <c r="C96" s="15" t="s">
-        <v>9</v>
+      <c r="C96" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B97" s="10">
         <v>1300</v>
       </c>
-      <c r="C97" s="16" t="s">
-        <v>14</v>
+      <c r="C97" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>103</v>
@@ -2523,15 +2520,15 @@
     </row>
     <row r="98" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B98" s="10">
-        <v>1300</v>
-      </c>
-      <c r="C98" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" s="3" t="s">
+        <v>2500</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D98" s="6" t="s">
         <v>104</v>
       </c>
       <c r="E98" s="1"/>
@@ -2543,8 +2540,8 @@
       <c r="B99" s="10">
         <v>2500</v>
       </c>
-      <c r="C99" s="18" t="s">
-        <v>47</v>
+      <c r="C99" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>105</v>
@@ -2558,8 +2555,8 @@
       <c r="B100" s="10">
         <v>2500</v>
       </c>
-      <c r="C100" s="12" t="s">
-        <v>5</v>
+      <c r="C100" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>106</v>
@@ -2568,15 +2565,15 @@
     </row>
     <row r="101" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B101" s="10">
-        <v>2500</v>
-      </c>
-      <c r="C101" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D101" s="6" t="s">
+        <v>6000</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" s="3" t="s">
         <v>107</v>
       </c>
       <c r="E101" s="1"/>
@@ -2588,53 +2585,53 @@
       <c r="B102" s="10">
         <v>6000</v>
       </c>
-      <c r="C102" s="12" t="s">
-        <v>5</v>
+      <c r="C102" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>108</v>
       </c>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B103" s="10">
         <v>6000</v>
       </c>
-      <c r="C103" s="14" t="s">
-        <v>8</v>
+      <c r="C103" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="B104" s="10">
-        <v>6000</v>
-      </c>
-      <c r="C104" s="16" t="s">
-        <v>14</v>
+        <v>5400</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B105" s="10">
         <v>5400</v>
       </c>
-      <c r="C105" s="14" t="s">
-        <v>8</v>
+      <c r="C105" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>154</v>
@@ -2643,58 +2640,58 @@
     </row>
     <row r="106" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B106" s="10">
         <v>5400</v>
       </c>
-      <c r="C106" s="12" t="s">
-        <v>5</v>
+      <c r="C106" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>155</v>
       </c>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
-        <v>128</v>
+        <v>53</v>
       </c>
       <c r="B107" s="10">
-        <v>5400</v>
-      </c>
-      <c r="C107" s="16" t="s">
-        <v>14</v>
+        <v>1000</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B108" s="10">
         <v>1000</v>
       </c>
-      <c r="C108" s="12" t="s">
-        <v>5</v>
+      <c r="C108" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="E108" s="1"/>
     </row>
-    <row r="109" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B109" s="10">
         <v>1000</v>
       </c>
-      <c r="C109" s="16" t="s">
-        <v>14</v>
+      <c r="C109" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>111</v>
@@ -2703,15 +2700,15 @@
     </row>
     <row r="110" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B110" s="10">
-        <v>1000</v>
-      </c>
-      <c r="C110" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D110" s="3" t="s">
+        <v>1900</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E110" s="1"/>
@@ -2723,23 +2720,23 @@
       <c r="B111" s="10">
         <v>1900</v>
       </c>
-      <c r="C111" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" s="2" t="s">
+      <c r="C111" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E111" s="1"/>
     </row>
-    <row r="112" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B112" s="10">
         <v>1900</v>
       </c>
-      <c r="C112" s="14" t="s">
-        <v>8</v>
+      <c r="C112" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>114</v>
@@ -2753,68 +2750,68 @@
       <c r="B113" s="10">
         <v>1900</v>
       </c>
-      <c r="C113" s="15" t="s">
-        <v>9</v>
+      <c r="C113" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>115</v>
       </c>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B114" s="10">
         <v>1900</v>
       </c>
-      <c r="C114" s="16" t="s">
-        <v>14</v>
+      <c r="C114" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E114" s="1"/>
     </row>
-    <row r="115" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="9" t="s">
-        <v>54</v>
+        <v>134</v>
       </c>
       <c r="B115" s="10">
-        <v>1900</v>
-      </c>
-      <c r="C115" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D115" s="3" t="s">
+        <v>7000</v>
+      </c>
+      <c r="C115" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D115" s="10">
+        <v>99999</v>
+      </c>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B116" s="10">
+        <v>4000</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E115" s="1"/>
-    </row>
-    <row r="116" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B116" s="10">
-        <v>7000</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D116" s="10">
-        <v>99999</v>
-      </c>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B117" s="10">
         <v>4000</v>
       </c>
-      <c r="C117" s="12" t="s">
-        <v>5</v>
+      <c r="C117" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>118</v>
@@ -2828,8 +2825,8 @@
       <c r="B118" s="10">
         <v>4000</v>
       </c>
-      <c r="C118" s="15" t="s">
-        <v>9</v>
+      <c r="C118" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>119</v>
@@ -2838,16 +2835,16 @@
     </row>
     <row r="119" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B119" s="10">
-        <v>4000</v>
-      </c>
-      <c r="C119" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>120</v>
+        <v>6500</v>
+      </c>
+      <c r="C119" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="E119" s="1"/>
     </row>
@@ -2858,11 +2855,11 @@
       <c r="B120" s="10">
         <v>6500</v>
       </c>
-      <c r="C120" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D120" s="4" t="s">
-        <v>105</v>
+      <c r="C120" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="E120" s="1"/>
     </row>
@@ -2873,40 +2870,40 @@
       <c r="B121" s="10">
         <v>6500</v>
       </c>
-      <c r="C121" s="12" t="s">
-        <v>5</v>
+      <c r="C121" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D121" s="7" t="s">
         <v>121</v>
       </c>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B122" s="10">
         <v>6500</v>
       </c>
-      <c r="C122" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D122" s="7" t="s">
+      <c r="C122" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B123" s="10">
         <v>6500</v>
       </c>
-      <c r="C123" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D123" s="3" t="s">
+      <c r="C123" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D123" s="7" t="s">
         <v>123</v>
       </c>
       <c r="E123" s="1"/>
@@ -2918,35 +2915,34 @@
       <c r="B124" s="10">
         <v>6500</v>
       </c>
-      <c r="C124" s="16" t="s">
-        <v>14</v>
+      <c r="C124" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="9" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="B125" s="10">
-        <v>6500</v>
-      </c>
-      <c r="C125" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E125" s="1"/>
+        <v>5800</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D125" s="10">
+        <v>99999</v>
+      </c>
     </row>
     <row r="126" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="9" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="B126" s="10">
-        <v>5800</v>
+        <v>4400</v>
       </c>
       <c r="C126" s="11" t="s">
         <v>12</v>
@@ -2957,29 +2953,15 @@
     </row>
     <row r="127" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="9" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="B127" s="10">
-        <v>4400</v>
+        <v>5900</v>
       </c>
       <c r="C127" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D127" s="10">
-        <v>99999</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B128" s="10">
-        <v>5900</v>
-      </c>
-      <c r="C128" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D128" s="10">
         <v>99999</v>
       </c>
     </row>
@@ -2988,19 +2970,18 @@
     <hyperlink ref="D24" r:id="rId1" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37053699&amp;forPersonCustId=3200" xr:uid="{76D85841-0E92-4011-A17D-A4C4F39B78A0}"/>
     <hyperlink ref="D25" r:id="rId2" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=25530467&amp;forPersonCustId=3100" xr:uid="{C9A79CA9-B167-443A-AB21-1EA20451173E}"/>
     <hyperlink ref="D26" r:id="rId3" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=27542090&amp;forPersonCustId=3100" xr:uid="{6D2A01E7-99B9-4DCA-8F10-0193BA4220F1}"/>
-    <hyperlink ref="D27" r:id="rId4" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37055482&amp;forPersonCustId=3100" xr:uid="{53D741C5-74C7-42B4-8631-E0FC11F4CAA7}"/>
-    <hyperlink ref="D44" r:id="rId5" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{22C1094A-0EAE-42D9-B543-021DD6A2C36F}"/>
-    <hyperlink ref="D45" r:id="rId6" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{7E462E08-4B0C-476D-AA36-E11FA80272FA}"/>
-    <hyperlink ref="D46" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{13B4A8AE-B629-42F9-B867-9E81A7263C7A}"/>
-    <hyperlink ref="D92" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{C28604FE-26D1-453D-8E55-BF4C270F28C4}"/>
-    <hyperlink ref="D93" r:id="rId9" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{E9917C5C-D5F0-4AD9-A2ED-472C92E6011C}"/>
-    <hyperlink ref="D111" r:id="rId10" display="http://puchakraborty.cm/" xr:uid="{02AFB277-C913-480D-BB5B-879E6BB17D14}"/>
-    <hyperlink ref="D21" r:id="rId11" xr:uid="{FCE7A3BF-4446-4E9F-83A0-11A360F0A079}"/>
-    <hyperlink ref="A73" r:id="rId12" tooltip="Optum Care Network - Idaho" display="javascript:void(0);" xr:uid="{90E131F6-422B-407C-B173-D7B05E9A01F6}"/>
-    <hyperlink ref="A81" r:id="rId13" tooltip="Optum Kansas City" display="javascript:void(0);" xr:uid="{ED7C1925-38C1-4B1C-BD55-4AC2E2B634E2}"/>
+    <hyperlink ref="D43" r:id="rId4" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=33993491&amp;forPersonCustId=3500" xr:uid="{22C1094A-0EAE-42D9-B543-021DD6A2C36F}"/>
+    <hyperlink ref="D44" r:id="rId5" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=31837442&amp;forPersonCustId=3500" xr:uid="{7E462E08-4B0C-476D-AA36-E11FA80272FA}"/>
+    <hyperlink ref="D45" r:id="rId6" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=37034624&amp;forPersonCustId=3500" xr:uid="{13B4A8AE-B629-42F9-B867-9E81A7263C7A}"/>
+    <hyperlink ref="D91" r:id="rId7" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=36963206&amp;forPersonCustId=3800" xr:uid="{C28604FE-26D1-453D-8E55-BF4C270F28C4}"/>
+    <hyperlink ref="D92" r:id="rId8" display="https://www.cozeva.com/new_settings?session=YXBwX2lkPXJlZ2lzdHJpZXMmY3VzdElkPTE1MDAmcGF5ZXJJZD0xNTAwJm9yZ0lkPTE1MDA&amp;person_id=40707817&amp;forPersonCustId=3800" xr:uid="{E9917C5C-D5F0-4AD9-A2ED-472C92E6011C}"/>
+    <hyperlink ref="D110" r:id="rId9" display="http://puchakraborty.cm/" xr:uid="{02AFB277-C913-480D-BB5B-879E6BB17D14}"/>
+    <hyperlink ref="D21" r:id="rId10" xr:uid="{FCE7A3BF-4446-4E9F-83A0-11A360F0A079}"/>
+    <hyperlink ref="A72" r:id="rId11" tooltip="Optum Care Network - Idaho" display="javascript:void(0);" xr:uid="{90E131F6-422B-407C-B173-D7B05E9A01F6}"/>
+    <hyperlink ref="A80" r:id="rId12" tooltip="Optum Kansas City" display="javascript:void(0);" xr:uid="{ED7C1925-38C1-4B1C-BD55-4AC2E2B634E2}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
PIH CU user change
</commit_message>
<xml_diff>
--- a/assets/CustomerDB.xlsx
+++ b/assets/CustomerDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wdey\PycharmProjects\Release-Team-Verification-Suite\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1442EABE-148A-4ABF-AEBB-ABAB4C567E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0104C815-AE2C-4F93-962A-CB123F11DC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,9 +297,6 @@
     <t>dmorales</t>
   </si>
   <si>
-    <t>Pih_jcoyne</t>
-  </si>
-  <si>
     <t>PIH_aacha</t>
   </si>
   <si>
@@ -526,6 +523,9 @@
   </si>
   <si>
     <t>MRTG_BCano</t>
+  </si>
+  <si>
+    <t>Pih_ktorres</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="2" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="10">
         <v>99999</v>
@@ -1109,7 +1109,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -1124,7 +1124,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -1139,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -1154,7 +1154,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -1169,7 +1169,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -1184,7 +1184,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="12" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="10">
         <v>6800</v>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="18" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" s="10">
         <v>6700</v>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="19" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B19" s="10">
         <v>7100</v>
@@ -1349,7 +1349,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="21" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21" s="10">
         <v>7500</v>
@@ -1379,7 +1379,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1619,7 +1619,7 @@
         <v>5</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E37" s="1"/>
     </row>
@@ -1649,7 +1649,7 @@
         <v>8</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E39" s="1"/>
     </row>
@@ -1664,7 +1664,7 @@
         <v>9</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E40" s="1"/>
     </row>
@@ -1679,7 +1679,7 @@
         <v>14</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E41" s="1"/>
     </row>
@@ -1829,7 +1829,7 @@
         <v>6</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E51" s="1"/>
     </row>
@@ -1844,7 +1844,7 @@
         <v>5</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E52" s="1"/>
     </row>
@@ -1859,7 +1859,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E53" s="1"/>
     </row>
@@ -1874,7 +1874,7 @@
         <v>9</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E54" s="1"/>
     </row>
@@ -1889,7 +1889,7 @@
         <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E55" s="1"/>
     </row>
@@ -1904,7 +1904,7 @@
         <v>6</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E56" s="1"/>
     </row>
@@ -1919,7 +1919,7 @@
         <v>5</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E57" s="1"/>
     </row>
@@ -1934,7 +1934,7 @@
         <v>14</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E58" s="1"/>
     </row>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="61" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B61" s="10">
         <v>5600</v>
@@ -1979,13 +1979,13 @@
         <v>5</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B62" s="10">
         <v>5600</v>
@@ -1994,7 +1994,7 @@
         <v>8</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E62" s="1"/>
     </row>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="71" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B71" s="10">
         <v>2800</v>
@@ -2135,7 +2135,7 @@
     </row>
     <row r="72" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B72" s="19">
         <v>1550</v>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="73" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B73" s="10">
         <v>6600</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="76" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B76" s="10">
         <v>5300</v>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="80" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B80" s="19">
         <v>1650</v>
@@ -2322,7 +2322,7 @@
         <v>5</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="E84" s="1"/>
     </row>
@@ -2337,7 +2337,7 @@
         <v>8</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E85" s="1"/>
     </row>
@@ -2352,7 +2352,7 @@
         <v>9</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E86" s="1"/>
     </row>
@@ -2367,7 +2367,7 @@
         <v>5</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E87" s="1"/>
     </row>
@@ -2382,7 +2382,7 @@
         <v>9</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -2397,7 +2397,7 @@
         <v>14</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E89" s="1"/>
     </row>
@@ -2412,7 +2412,7 @@
         <v>6</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E90" s="1"/>
     </row>
@@ -2427,7 +2427,7 @@
         <v>5</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E91" s="1"/>
     </row>
@@ -2442,7 +2442,7 @@
         <v>14</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E92" s="1"/>
     </row>
@@ -2457,7 +2457,7 @@
         <v>6</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E93" s="1"/>
     </row>
@@ -2472,7 +2472,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E94" s="1"/>
     </row>
@@ -2487,7 +2487,7 @@
         <v>8</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E95" s="1"/>
     </row>
@@ -2502,7 +2502,7 @@
         <v>9</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -2517,7 +2517,7 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E97" s="1"/>
     </row>
@@ -2532,7 +2532,7 @@
         <v>6</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E98" s="1"/>
     </row>
@@ -2547,7 +2547,7 @@
         <v>47</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E99" s="1"/>
     </row>
@@ -2562,7 +2562,7 @@
         <v>5</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E100" s="1"/>
     </row>
@@ -2577,7 +2577,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E101" s="1"/>
     </row>
@@ -2592,7 +2592,7 @@
         <v>5</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E102" s="1"/>
     </row>
@@ -2607,7 +2607,7 @@
         <v>8</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E103" s="1"/>
     </row>
@@ -2622,13 +2622,13 @@
         <v>14</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B105" s="10">
         <v>5400</v>
@@ -2637,13 +2637,13 @@
         <v>8</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B106" s="10">
         <v>5400</v>
@@ -2652,13 +2652,13 @@
         <v>5</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B107" s="10">
         <v>5400</v>
@@ -2667,7 +2667,7 @@
         <v>14</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E107" s="1"/>
     </row>
@@ -2682,7 +2682,7 @@
         <v>5</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E108" s="1"/>
     </row>
@@ -2697,7 +2697,7 @@
         <v>14</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E109" s="1"/>
     </row>
@@ -2712,7 +2712,7 @@
         <v>6</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E110" s="1"/>
     </row>
@@ -2727,7 +2727,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E111" s="1"/>
     </row>
@@ -2742,7 +2742,7 @@
         <v>8</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E112" s="1"/>
     </row>
@@ -2757,7 +2757,7 @@
         <v>9</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E113" s="1"/>
     </row>
@@ -2772,7 +2772,7 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E114" s="1"/>
     </row>
@@ -2787,13 +2787,13 @@
         <v>6</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B116" s="10">
         <v>7000</v>
@@ -2817,7 +2817,7 @@
         <v>5</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E117" s="1"/>
     </row>
@@ -2832,7 +2832,7 @@
         <v>9</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E118" s="1"/>
     </row>
@@ -2847,7 +2847,7 @@
         <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E119" s="1"/>
     </row>
@@ -2862,7 +2862,7 @@
         <v>47</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E120" s="1"/>
     </row>
@@ -2877,7 +2877,7 @@
         <v>5</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -2892,7 +2892,7 @@
         <v>8</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E122" s="1"/>
     </row>
@@ -2907,7 +2907,7 @@
         <v>9</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E123" s="1"/>
     </row>
@@ -2922,7 +2922,7 @@
         <v>14</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E124" s="1"/>
     </row>
@@ -2937,13 +2937,13 @@
         <v>6</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B126" s="10">
         <v>5800</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="128" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B128" s="10">
         <v>5900</v>

</xml_diff>